<commit_message>
Get daily reddit data: Tue Jan 28 08:10:50 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_02.xlsx
+++ b/data/collected_data/2025_02_02.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C502"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3423 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1ibwewd</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>The set I did yesterday and I love it so much!</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zoiux4tcuofe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1ibvu4k</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Valentine's set</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibvu4k</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1ibucya</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Is this mold?</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/31lluwwd5ofe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1ibugyy</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Nail question … what is the difference between all these options?</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qwstve9m6ofe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1ibuugu</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>A Valentine's inspired set</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6huynxuaofe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1ibv20e</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Nail health</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ibv20e/nail_health/</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1ibvfs8</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>valentine’s day nails 💗</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bwgww61uhofe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1ibv37m</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>How to come to terms with a manicure?</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibv37m</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1ibv16w</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Who doesn't love a good multichrome moment??</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jlxaho12dofe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1ibue0p</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Very cutesy, very demure? 🤭💅</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibue0p</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1ibu59l</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>A set so beloved, I kept them</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibu59l</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1ibtv20</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>theme: snakes 🐍 which set do you like the most?</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibtv20</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1ibt7wi</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Did my nails for the first in forever!</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibt7wi</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1ibtq8v</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Can I do this?</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ibtq8v/can_i_do_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1ibt6lb</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Which shape looks good on my hand?</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibt6lb</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1ibt13c</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Tried my best to fix lol lol</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibt13c</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1ibsz8d</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Really digging my new set!</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kq9xn1qarnfe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1ibsvs5</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Should I “debulk”</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibsvs5</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1ibstav</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Missing my oval shape</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibstav</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1ibqsxh</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Need advice</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpcj5cu67nfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1ibs2sb</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>My Chinese New Year 2025 inspired nails 🧧</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibs2sb</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1ibr493</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>BTArtbox Question</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ibr493/btartbox_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1ibrm5q</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Birthday Set 🎂</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ffnsql2fenfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1ibrh5b</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Valentine nails and we added my fiancés initial to a locket design ❤️</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b9djhie5dnfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1ibrgwg</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>New Nail Tech</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zjtpn1c3dnfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1ibr8j3</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Valentine nails💅💘💋💖❣️💌</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggad00q0bnfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1ibr56x</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>I’m really proud of my design today. I’m improving my lines I think</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gg2b76w6anfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1ibqzfd</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Sad image🤡</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58iyi96r8nfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1ibqw0w</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Tried the clear top coat over matte top coat design trick</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k106cl2x7nfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1ibqpef</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails ❤️</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgbz3d496nfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1ibqc88</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>first time trying nail art ☺️</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9mhbrp43nfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1iblzcs</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Clean and Fresh nail colour recommendations?</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0i2e2xrm3mfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1ibq9xw</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Vday nails 💘</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0tav0otj2nfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1ibq8a6</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>winter blue</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibq8a6</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1ibq5bu</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Nail Breakage</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibq5bu</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1ibpqnd</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Please help. What do I do?</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibpqnd</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1ibm576</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Why do my nails brake off???</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibm576</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1ibp8wx</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Does this color look okay with my pale complexion ?</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f9t3tyaltmfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1iboaqv</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Just removed builder gel after a year</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iboaqv/just_removed_builder_gel_after_a_year/</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1ibnznk</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Hi, how are you? What do you think of my natural nails? I wanted to recreate Hailey Bieber style ☺️ Do you like it?</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rc467tp6jmfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1ibnr4o</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>I love this shifty color!</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ibnr4o/i_love_this_shifty_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1ibno0f</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>How do these look please be honest</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dycqetzkgmfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1ibnbuu</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Wondering why water is an ingredient in nail oils.</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ibnbuu/wondering_why_water_is_an_ingredient_in_nail_oils/</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1ibn9f5</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Lifting nails; Can I get a refund??</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibn9f5</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1ibn683</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Queen of Hearts</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibn683</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1ibmzzn</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>15 day retention for press-on nails is crazyyy ♥️</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibmzzn</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1ibmmhy</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>does anyone have any simple nail art ideas for these?</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u34h0x6j8mfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1ibm7p6</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibm7p6</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1ibm4xf</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Cute pastels 💛💜💗💙</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5rwap1zs4mfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1ibl3gj</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Curved red tips, with gold spark accent</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g1zodya7xlfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1ibkxxu</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>third nail set on myself (2nd and 3rd slide for dog)</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibkxxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1ibkj7t</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Nail shape advice please?!</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/adz400z4tlfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1ibgvph</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Been Doing my Own Nails for Over a Year Now!!</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibgvph</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1ibkqp2</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Black heart 🖤</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ill0wuvmulfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1ibkkhb</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Looking for firm builder gel</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ibkkhb/looking_for_firm_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1ibkjf6</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>absolutely gagged by this set</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibkjf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1ibjy21</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>pink + black</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibjy21</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1ibjqrg</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Are my nails nice?</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2uedfahnlfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1ibjdg9</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Found a new place and excited!</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9elue2irklfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1ibiwyu</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Did these on myself 🥰</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/co5sk20ehlfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1ibisbu</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>I want ideas to improve my gel x valentines set</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bflix7vcglfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1ibiro9</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Valentine 💘 nails</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibiro9</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1ibicd0</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Can I get nail beds like a hand model?</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ibicd0/can_i_get_nail_beds_like_a_hand_model/</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1ibi5zv</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Fire Emblem Fates Hinoka as Stained Glass Painting Nail Art!</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibi5zv</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1ibi25x</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Love my new set</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7f09l4l4blfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1ibhyg9</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Obsessed with Gel X Nails</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xh2l9erdalfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1ibhyft</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Love my nails! 💅</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1b52godalfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1ibhvkw</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Literally my favourite nails that I’ve ever had!! Rain drops and flower designs!!🧚🏻💕</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibhvkw</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1ibhmcr</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Cracked gel-x/builder gel nail</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibhmcr</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1ibgw74</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>obsessed ✨</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0da4pjlt2lfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1ibf8ew</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Pink and white variations</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ibf8ew/pink_and_white_variations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1ibgo83</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Obsessed 💖</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frn90f081lfe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1ibgo42</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>To long ? I love the look and design but .. something feels off ? I like to get acrylics regularly so any tips on how to get colors or designs would be great.</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibgo42</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1ibgffr</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Gel removal advice?</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avd33ysgzkfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1ibg84c</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Some Manicures I’ve gotten on my natural nails 🌸</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibg84c</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1ibfnax</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Valentines nails + dry hands ft my jewelry</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0seesdv0ukfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1ibfkfb</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Jumped on the chrome train!</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zyjhtf0htkfe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1ibf3fa</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Practicing nail art! Another LNY set 🐍🧧</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibf3fa</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1ibeirk</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Chinese New Year Nails</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibeirk</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1ibecbg</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>My newest minimalist claws</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibecbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1ibe874</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Talk me off the ledge (of picking my nails off)</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibe874</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1ibe44m</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>I went to a new nail salon and I love the color but feel like it could be shaped better. Spent 52$</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/maatqnk4jkfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1ibdy63</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Pay is $50 for Russian manicure. Does it looks worth it?</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0kh2s981ikfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1ibdawf</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Question about Castor Oil: do you mix it with something else or just apply it on the nail?</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ibdawf/question_about_castor_oil_do_you_mix_it_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1ibd22z</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Red Bottoms</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibd22z</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1ibd1p7</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Valentine's Day</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pzkl737hbkfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1ib1q2q</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>remake of a set from a year ago</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ib1q2q</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1ibcwuj</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>A little gold to welcome the Lunar new year ✨✨✨</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibcwuj</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1ibc5fa</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Chinese New Year 🧧 Year of the Snake 🐍 Nail Design 💅</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibc5fa</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1ibbtpm</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Doing my own nails for the first time</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22cbm18d2kfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1ibbsg6</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>First time with polygel</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibbsg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1ibboi3</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Early Valentines Set</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eu7wm03c1kfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1ibbmiy</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Are these too long?</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibbmiy</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1ibbccq</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Best cheap Electric nail file</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ibbccq/best_cheap_electric_nail_file/</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1ibb6tv</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Newly Departed 💔 - Velvet Rose by Mooncat</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibb6tv</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1ibayxx</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>obsessed doenst even cover it, my first time at an independent tech</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibayxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1ibawcy</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>very basic… I really want to learn how to do nail art</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zy8ts3imvjfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1ibausl</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Valentine nails :)</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibausl</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1ibauex</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Some of my press ons since last April</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibauex</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1ibarq0</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Pretty in magenta</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xr65n6klujfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1ibvsng</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>ISO intense blurple with hot pink shimmer</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/toddsacbmofe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1ibvkcu</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>How do you stop it from chipping</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o0z3bj8djofe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1ibv5uy</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Orly Spring Collection for Color Pass</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibv5uy</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1ibv0qi</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Does anyone have iridescent glitter topper recommendations that look like this?</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5hn0p1axcofe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1ibujzk</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Should I be concerned about contact dermatitis?</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ibujzk/should_i_be_concerned_about_contact_dermatitis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1ibtxxm</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Broke my arm and leg but I can still paint my nails</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/phwmfe151ofe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1ibthlx</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>pastel blue velvet nails</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibthlx</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1ibtdsz</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Looking for a cool toned brown shimmer</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/635pf8c9vnfe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1ibtdnv</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Psilocybin - Clionadh</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uszg85m7vnfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1ibsxc4</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Everyone always talks about Cock A Doodle Doom… but what about Chicago Fire? 🔥</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibsxc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1ibsmst</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Two different toppers</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibsmst</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1ibru5f</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>January PPU arrived today!</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibru5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1ibrl52</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Clionadh haul swatch</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hhi9wpa5enfe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1ibrk4h</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Wasn't feeling it until I caught it in the Sun</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibrk4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1ibrdmb</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Never Tide Down</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibrdmb</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1ibr8r9</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Lyn B’s shimmers are to die for</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibr8r9</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1ibqzag</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Mooncat - Fake Halo 😇</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibqzag</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1ibqcmk</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Has this happened to anyone else?</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibqcmk</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1ibpdpt</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>I have a problem…</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibpdpt</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1ibmzfk</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>How long can I expect Clionadh to still have Psilocybin &amp; sibs?</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ibmzfk/how_long_can_i_expect_clionadh_to_still_have/</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1ibnvz8</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>index finger need TLC</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ibnvz8/index_finger_need_tlc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1ibnp36</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>My first PPU</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/seu5scgtgmfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1ibn7kx</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Did I dupe myself?</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ibn7kx/did_i_dupe_myself/</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1ibn56i</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Dreamy sunset skittle</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibn56i</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1ibn4su</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Happy Lunar New Year!</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oruimk9dcmfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1ibmuk2</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Dollar store valentines mani 💕</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibmuk2</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1ibms97</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Holo Taco 'Freezer Burn' got a workout!</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c0l6i19r9mfe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1ibmqjz</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Any regular polish brand recommendations for stamping?</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ibmqjz/any_regular_polish_brand_recommendations_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1ibm8ya</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Are my cuticles seriously injured?</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibm8ya</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1ibm7gz</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Why do my nails brake off?</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibm7gz</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1iblpvp</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>First BCB Lacquers!</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iblpvp</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1iblpj3</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>happy lunar new year 🧧</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iblpj3</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1ibl9l9</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>What polish brands do you recommend?</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ibl9l9/what_polish_brands_do_you_recommend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1ibl2lp</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Mooncat Triceratops is a stunning moody shade!</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibl2lp</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1ibkus6</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>It's always the polishes you expect the least from</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibkus6</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1ibkrtu</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Opal attempt in a jelly sandwich</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibkrtu</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1ibkj0m</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>ABCs of polish!!! Two for one (kinda) Y is for Yapa Beauty and Z is for Zoya in</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibkj0m</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1ibk6o7</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Silly ways we broke a nail</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ibk6o7/silly_ways_we_broke_a_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1ibjam9</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Out cold by Emily de Molly vs ILNP Songbird</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ibjam9/out_cold_by_emily_de_molly_vs_ilnp_songbird/</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1ibiyz5</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>ILNP Pink Lemonade has my heart this month.</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibiyz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1ibhdsp</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>ILNP Salem vs Mooncat Access Denied</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ibhdsp/ilnp_salem_vs_mooncat_access_denied/</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1ibh4xp</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Midnight Owl ✨</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibh4xp</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1ibguxg</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Mooncat Drown my Demons. Had to take a break to enjoy it in the sunlight.</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h2w0elzj2lfe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1ibgtog</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Another polish I bought for February but couldn’t wait to wear: Emily de Molly “Have My Heart” 😍</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibgtog</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1ibgjlt</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>What's a polish name that you have a hard time pronouncing 🤔</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9f0oq25a0lfe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1ibg8vp</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Trying a baby almond - love the shape but I keep scratching myself!</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ogi6yji6ykfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1ibg5ya</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Polished for Days What Dreams Are Made Of</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibg5ya</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1ibg5ty</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Stop staining please!</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ibg5ty/stop_staining_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1ibfn0b</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Help finding dupes for Holo Taco Life In Plastic and Be Kind Rewind</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ibfn0b/help_finding_dupes_for_holo_taco_life_in_plastic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1ibf8jo</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Can I DUPE IT? (A Tribe Called Quest: YES YOU CAN!)</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vrjag9z4rkfe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1ibet87</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Super Bowl bound!</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n8y1pv53okfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1ibekmd</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>In the doldrums of winter I crave layers of rainbows</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibekmd</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1ibeitd</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Decided to get Holo Taco “Not Pressed” since it’s retiring, and I  genuinely cannot decide if I love or hate it 😅 wearing “Not Pressed” and “Matte Taco.”</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79hpisv1mkfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1ibe5r6</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Mastermind by Cadillaquer</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ibe5r6/mastermind_by_cadillaquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1ibdaj9</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>The perfect manisnack</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ewq0bw9dkfe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1ibd49k</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>First time using stamps</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1lskhi0ckfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1ibcqfh</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Mooncat Queen of The Dead dupe?</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ibcqfh/mooncat_queen_of_the_dead_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1ibcib2</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Stringy top coat</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ibcib2/stringy_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1ibbzmb</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Jojoba oil in a dropper</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/obwbpaqm3kfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1ibbxu0</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Dollar Tree OPI</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2u4urjd93kfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1ibbi29</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Anyone have non-PVB basecoat recommendations if I love Essie's First Base?</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ibbi29/anyone_have_nonpvb_basecoat_recommendations_if_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1ibb84p</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>They match the Dr Pepper can lol</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43h1ywg4yjfe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1ibawn5</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Question about Polished for Days polishes</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ibawn5/question_about_polished_for_days_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1ibar30</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>One Year of Growth</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibar30</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1ibamtb</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>🪙🎮Mario Part III⭐️🍄</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibamtb</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1iba0qr</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>How to get this radial ombré effect?</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iu9rp3efojfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1ib7utn</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>I’m liking this a lot by itself</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ib7utn</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1ib60fg</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ib60fg/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1ib5y5f</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Another day, another mani I can't stop looking at</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ff0sdprmpife1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1ibwoav</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Anyone rate the Temu nail stickers ? Do they last ?</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ibwoav/anyone_rate_the_temu_nail_stickers_do_they_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1ibw0rj</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>I love how sparkly it is.</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aa2uccq3pofe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1ibvu6g</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>It worked!</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i8lxnb8umofe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1ibvtu0</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Happy Aquarius Season 🏺🌊</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y00zo87qmofe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1ibvl8a</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Cute &amp; funky</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibvl8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1ibvgnz</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>my first try at nail art !</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ff4ylo4iofe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1ibsipc</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Simple set I did a while back. The itty bitty flowers are my fave to do in the summer/spring</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bjbw2ubomnfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1ibrvec</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Crystal reference suggestions welcome.</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5xf6egtrgnfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1ibr1g0</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Can u tell I love junk nails?</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibr1g0</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1ibpd6x</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>y’all are so freaky, I thought you’d enjoy these nails I did for Halloween</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibpd6x</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1ibnypu</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Hyperealistic human claws that I hand paint &amp; sculpt with polygel</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibnypu</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1ibngvg</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Not proud of these nails, but I thought I’d share</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibngvg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1ibn7de</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>some of the sets i’ve made so far :)</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibn7de</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1ibmfwe</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Glossy Top Coat Recommendations?</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ui7awr47mfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1iblzry</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Hand-painted Iris from the upcoming movie Companion. Her eyes go white like in the movie!</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iblzry</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1ibltx2</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>🦈 shark week</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibltx2</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1ibljna</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Starting to practice nail art</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o4voeu9f0mfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1ibldpt</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Pink</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7fr7h5pazlfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1ibkzfp</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Tried my airbrush for the first time</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibkzfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1ibi6s6</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Fire Emblem Fates Hinoka as Stained Glass Painting Nail Art!</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibi6s6</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1ibhpgk</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Valentine’s Day set</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nlkzcm8l8lfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1ibh46f</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Any tips on getting my art precise</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jprzi9bb4lfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1ibgykp</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>I leave you a little picture of my nails, could you give me some ideas to make them in different colors? Thanks</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4n8mp1a3lfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1ibfbx7</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>V-Day Nail Art</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ar7omfxtrkfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1ibelc7</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Chinese New Year Nails</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibelc7</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1ibej4l</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Practicing nail art! LNY set 🐍🧧</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibej4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1ibebuw</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Eye</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibebuw</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1ibbkl2</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Kuromi nails 💜</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tppo3hyn0kfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1ib8mkt</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Out of my comfort zone</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ghyjxb8djfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1ib5zn8</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Feeling the pink for Valentine’s Day 💖💖</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/95nboz00qife1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1ib3xc2</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ib3xc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1ib3hed</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Valentine's day nails</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ib3hed</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jan 29 08:10:42 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_02.xlsx
+++ b/data/collected_data/2025_02_02.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C502"/>
+  <dimension ref="A1:C715"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8967,6 +8967,3627 @@
         </is>
       </c>
     </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1icotgk</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>How to make the shape more sharp?</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4zxobbp72wfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1icosse</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Squid Game set</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0gjp5cy1wfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1icnr0w</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Just got this set and love it ♥️♥️</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icnr0w</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1icnpjt</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Second attempt at stained glass vampy nails</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/525hz2vonvfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1icncop</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Pretty in pink (baby boomer)</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t22f7hafjvfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1iclff9</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Filling in a severely ridged nail?</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2bg96vtyufe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1icmwaq</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>1st jan- 29th jan</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/60x76gr7evfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1icmj4v</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Press Ons I Picked Up Today!</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vrt5ika9avfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1icmbwq</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Obsessed w/my nails</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvntv6638vfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1iclui5</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Builder gel on natural nails</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iclui5</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1icltl4</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Feeling yellow💐✨</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icltl4</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1icl5iu</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Which shades of nailpolish would suit me?</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oum0jj2zvufe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1ickj2n</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Gel allergy press on precautions</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ickj2n/gel_allergy_press_on_precautions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1ickf06</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Roman Mosaic Nails!</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ickf06</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1ickz4g</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Little snakes for lunar new year 🐍🐍🐍</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s635dbcduufe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1ickpny</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>I was encouraged to wear short nails. The result was a subtle and elegant design.</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxmykavwrufe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1ickoid</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Graffiti vibes on my nails 🖤✨</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d1qsr13jrufe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1icjtac</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Rude customers…</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icjtac</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1icjdnu</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>So I’ve been doing my nails for a few months now and no matter what they’re super thin and break and last a week max what would be the longest lasting at a salon maybe acrylic overlay? Also color ideas?</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icjdnu</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1icjd7y</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>No acrylic</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yii03vzdfufe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1icj2y9</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>💕💕💕</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ejk6bttcufe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1icj2kq</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Set my friend did 🍏</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icj2kq</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1icj14y</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Best glue for my  Sailor Moon nail set ?</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjg28lxdcufe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1icizu7</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Looking for this color or something close to it</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q4sw1jr2cufe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1icix0k</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Why aren’t there skin fully around my nails? Can I revert it, or is it normal?</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icix0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1icis1a</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Recent nail sets I’ve done for myself and some clients!</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icis1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1icipmn</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>looking for the nail of this aesthetic/tutorials</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1icipmn/looking_for_the_nail_of_this_aesthetictutorials/</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1icidcg</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Nail Removal and Refund</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1icidcg/nail_removal_and_refund/</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1icicre</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Got these done today 💗</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1noiwsof6ufe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1icho4w</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>First time doing gel manicure</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dk8z98ai0ufe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1ichgsp</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Aurura effect natural polish</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ichgsp/aurura_effect_natural_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1ichdpp</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>combo of 4 different nail sticker sheets… I couldn’t decide</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ocv7yoqyxtfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1ich7lp</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>🍒✨</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mw1u4vpjwtfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1icgpjh</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>just wanted to share the birthday set i did for my beautiful friend!</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4p9yevtgstfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1icgnmp</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Valentines nails💌</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psrzust0stfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1icglpu</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>It's GAlinda to you 🦋</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9eqtm3klrtfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1icgext</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>DIY Newbieee</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bwo95rnwptfe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1icgf5w</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>My fav I miss it</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icgf5w</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1icgcb3</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Made my nails myself! 🩷</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icgcb3</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1icfm6j</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>my top coat looks like it sells crqck to other top coats</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rf7ylfdsjtfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1icfg71</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Nail damage</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0rkoeihitfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1icfhb8</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Glitter. Everywhere</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icfhb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1icffo9</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>DIY Kokoist Builder Gel</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icffo9</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1icfev0</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>what shape fits my hands best?</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icfev0</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1icfchd</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Today's color!</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g886s1gohtfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1icf9az</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>6 months with my nail tech</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icf9az</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1icerqb</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>A classic red on gel-x!!</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r9cq7h65dtfe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1icen3l</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>How do I take off superglued press ons??</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1icen3l/how_do_i_take_off_superglued_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1icem7l</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Nail Journey - see comments. Which shape?</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icem7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1icekc2</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>I’m a guy who wants my first set.</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o5qswpmkbtfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1icegos</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Line running along my nail</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dknonwjsatfe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1iced38</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Bubbles under gel—bad or okay?</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qommfctz9tfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1icdwbp</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>✨freshies✨</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icdwbp</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1icds4f</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>These are just press ons, i love them so bad thoughhh</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icds4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1icdi1x</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Self taught 💅🏻🤍</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8r11vgmi3tfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1icdfyw</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>bumpy/curly nails help</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1icdfyw/bumpycurly_nails_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1icddlc</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Any gel x tips?</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qr7m4iqk2tfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1icd5it</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Today I was babysitting a 4 year old and she did my nails lol so cute</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/au7w8ymv0tfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1iccvlh</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Charms</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/005u8utuysfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1icc9dl</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>First sets I’ve ever done!</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icc9dl</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1icbdbi</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>I hate my nails</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icbdbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1icbsqb</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Why do dots on my gel polish appear?</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gliv0aixqsfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1icbka8</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Pink thermal 💗🩷</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icbka8</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1icbgcs</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>New press-on for New Year</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icbgcs</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1icb4h1</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Is this too much?</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xexxlz2ylsfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1ica72c</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Valentines Nails</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ica72c</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1ic9iwc</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>new set of press ons! obsessed</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic9iwc</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1ic9138</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Festive, Minimal, &amp; adorable! 🥰</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic9138</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1ic9116</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Valentine's Day nails 🩷</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o49he8e07sfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1ic8ps1</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Dilemma: gel and acrylics only last about a week on my nails</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ic8ps1/dilemma_gel_and_acrylics_only_last_about_a_week/</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1ic8mxe</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>My dispatcher is becoming a nail tech</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic8mxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1ic7xzh</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Simple Valentine’s Set</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggnymcd5zrfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1ic7n28</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Pink and French Tip</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dk45d6kzwrfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1ic7fpg</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>When should I take off my acrylic nails?</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic7fpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1ic7fxo</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Good quality, awful conversation nail tech</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ic7fxo/good_quality_awful_conversation_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1ic787a</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Valentines chrome nails 💕</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic787a</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1ic7732</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>French Tip with Flowers</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic7732</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1ic6ae2</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Colored French nails?</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ic6ae2/colored_french_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1ic6qzy</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Fresh manicure for Valentine's Day</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic6qzy</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1ic5ngm</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Can anyone tell me what the name of the powder is?</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z1th53mkirfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1ic63r7</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>not happy with biab</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dr91w9zxlrfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1ic6fa3</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Oval or square?</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic6fa3</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1ic69wc</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Pink and glitter 💖</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hzgfid65nrfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1ic667y</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>My minimalist valentine's nails</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pf19u27gmrfe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1ic5ffi</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>MOONCAT - The Sea Between Us</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic5ffi</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1ic5aot</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Blue or red?</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic5aot</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1ic53a0</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Natural nails 💅</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic53a0</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1ic4xgy</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>New color!</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rmi8ug44drfe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1ic4wcc</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Holographic polishes are gorgeous</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic4wcc</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1ic4pys</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>I cant add enough gems! 🎀💖✨</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic4pys</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1ic4o5z</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Love new nail days</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic4o5z</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1ic4m0l</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Did a red French</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic4m0l</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1ic4fv2</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>What is a substitute for gel x?</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ic4fv2/what_is_a_substitute_for_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1ic4aax</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>My latest DIY set! 🦋</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z07y7ma78rfe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1ic3r3s</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Ayuda!/ Advice, please!</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ic3r3s/ayuda_advice_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1ibvvmu</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>To those who work fast food, how do you keep your nails healthy?</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ibvvmu/to_those_who_work_fast_food_how_do_you_keep_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1ic346a</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>It is almost mocha mousse nails</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic346a</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1ic2yzq</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>I’ve been Glinda-fied 🫧🪄💓</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic2yzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1ic2vlu</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Victoria Vynn</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ic2vlu/victoria_vynn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1ic2blv</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Any advice on how to improve my manicure?</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic2blv</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1icood6</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Ethereal Lacquer Candlelight</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icood6</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1ico4oo</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>The black glitter polish with a secret ✨🌈🖤</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ico4oo</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1icnxer</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>ILNP Addiction</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yjr51xqeqvfe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1icnv6d</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Lai See Inspired nails</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxzy9b1opvfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1icnqil</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Red and gold for Chinese New Year 🧧✨</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icnqil</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1icnl2f</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Bee’s Knees BG3 collection</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1icnl2f/bees_knees_bg3_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1iclymk</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>a brief visit with ghosts</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iclymk</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1icljgl</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>pt. 1/2 of my blue collection—these are my glitters and shimmers! 🔵✨what other sparkly blues do I need to add to my collection? cremes next!</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icljgl</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1iclg8i</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>ILNP bulletproof symphony vs MC star destroyer - with og swatch to show how ILNP has faded over time</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvo3g3vwyufe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1iclbgk</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>*faded* ILNP bulletproof symphony vs brand new MC star destroyer</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5rfix39jxufe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1icl0wt</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Dupe for Psionic by Phoenix Indie Polish?</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icl0wt</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1ick51v</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Super proud of this one. First attempt at shaping and cuticle execution 🌷</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ick51v</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1icjpkk</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>So I’ve been doing my nails for a few months now and no matter what they’re super thin and break and last a week max what would be the longest lasting at a salon maybe acrylic overlay? Also color ideas?</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icjdnu</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1icjajs</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Seen this video some months ago and asked for the color she was wearing and got no reply. Please anyone help me find this color❤️</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j72txj9qeufe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1icivr5</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>🌸 Mani from the new OPI Spring 2025 line</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icivr5</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1iciumy</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Full Scream Ahead 🗣️</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iciumy</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1icipaa</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Roman Mosaic Nails!</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icipaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1icimvu</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Got these today 💗</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9ptabkx8ufe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1icifco</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Celebrating Year of The Snake 🐍</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icifco</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1icid7a</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Kbshimmer For The Pun Of It is delightfully shifty!</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/agbgxvuj6ufe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1ici3ag</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>indie brands from etsy, part 1: ChromaVerse Polish</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ici3ag</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1ichush</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Relaxing muted teal… ❄️🌲</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ichush</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1ichkdv</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Extra Bottle Questipn</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ichkdv</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1ichfmy</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Holo Taco has so many different kinds of base coats! Is there any that is more recommended? Thanks!</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ichfmy/holo_taco_has_so_many_different_kinds_of_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1ichahh</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Milk Glass: my nails but better</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/atdrhws7xtfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1ich0nf</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>$10 Facebook Marketplace haul 💕</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ich0nf</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1icgzq0</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Voted Mooncat's ugliest polish 😭</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icgzq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1icgnuq</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>⭐️ STARS⭐️</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icgnuq</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1icgk62</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>so sad &amp; bummed</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1icgk62/so_sad_bummed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1icgjbi</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Distracting in every light...</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icgjbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1icgj7b</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>First Thermal!</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icgj7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1icghmh</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Mooncat Pink Piglet 2.0</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icghmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1icgfyt</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>BKL, Binding + I Invoke Thee 🔮</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icgfyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1icfigc</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Severance Manicure</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s61jm6ozitfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1iceg18</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Chrome powder immediately activates my lizard brain 🤤</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0a3ox44natfe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1icedyj</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>My nail desk is looking a bit witchy tonight 🧙‍♀️</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icedyj</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1icdsny</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Stained glass roses 🌹</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icdsny</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1ica96s</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Why does my finger nail how these bubbles or whatever in them???</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5vhgfetkfsfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1iccces</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Unknown colour name</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yx42od9yusfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1icdbc0</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Snowdrift mani - petals for a narcissist and celestial lights ❄️</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w01yh1k32tfe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1icd0qg</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>You can use any magnetic polish as a topper if it is sheer enough</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m4jaslqkzsfe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1icczy3</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Got inspirer by my Arizona green tea 🌸</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icczy3</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1iccyfp</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>First empty bottle</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydek8vqfzsfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1iccxfj</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Looking for the ultimate milky nude nail polish</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrj9tpm8zsfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1iccu1o</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Winter shorties 🖤</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/37cpzzvdysfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1icc05g</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>What Essie color is this?</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4k83gjvhssfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1icbwwu</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Help me find this chrome colour!!</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icbwwu</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1icbwfs</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Are mooncat bottles still breaking?</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1icbwfs/are_mooncat_bottles_still_breaking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1icbw30</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>ILNP Skye 🤩</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qilkt7tmrsfe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1icbv5r</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Stained Glass Windows</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4aywl86frsfe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1icamo3</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>GPL - Courteous Clairvoyant (prototype)</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icamo3</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1icagdx</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Kitty cat manicure</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icagdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1icacv0</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>ILNP Sleighbells is my most favorite nail polish ever 🩶</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icacv0</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1ic9vm2</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Chrome base with chrome design? (Isolated chrome on chrome?)</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ic9vm2/chrome_base_with_chrome_design_isolated_chrome_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1ic91h7</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Jan PPU - Psyche Minerals “Glittering Gala”</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j6mltz527sfe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1ic8ev7</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>I feel like hot trash but at least my nails look good 🤧</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/il04f7sk2sfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1ic8645</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Shout out to my 10+ year old bottle of OPI Crackle topper 😍😍 Remember when this finish had us in a choke hold??</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dj815x2t0sfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1ic7ow1</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>aaaaand this is why I take Reddit suggestions seriously 😍</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic7ow1</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1ic7c86</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>GLL for Chinese New Year</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic7c86</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1ic6z1i</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>emotional support 🌮</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic6z1i</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1ic6vff</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Cracked - Sweeter The Juice</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9iedibydrrfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1ic6odf</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Psilo-self care day</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic6odf</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1ic60sk</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>The many shades of bluebell😍</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic60sk</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1ic5tjn</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Red in Paris</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/jsGO2Rr</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1ic5hsl</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Essie Gilded Galaxy</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic5hsl</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1ic5fxk</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>MOONCAT - The Sea Between Us</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic5fxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1ic5bkc</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>The Moon - my first UV-reactive polish :3</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic5bkc</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1ic56n2</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Cirque on Amazon?</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ic56n2/cirque_on_amazon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1ic5585</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Loving this color and question</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic5585</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1ic5261</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Arcana Lacquer magnetics!</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic5261</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1ic4xiq</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>My first mattes in years</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic4xiq</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1ic4way</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>💀🖤Goth Glam🖤💀</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic4way</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1ic4v01</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>I ♥️ linear holo and linear holo ♥️ me</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/teossr8mcrfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1ic4g1z</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>90's Arcade Carpet Vibes</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic4g1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1ic494g</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Cadillacquer Hug the Dog &amp; ILNP Copper Top</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jwnm8r4y7rfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1ic3z9l</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>I heard we express ourselves here</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic3z9l</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1ic31mt</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Golden/Copper mani shining in day light✨😍</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/71ax45gayqfe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1ic2tu4</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>This week’s golden/copper mani in daylight✨🌟✨🥰</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic2tu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1ic2m05</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Glass nails video tutorial</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gtkpjr8fuqfe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1ic2bto</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>I’ve been a nail biter all my life and my nails are the longest they ever been. How do I relearn to do stuff??</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ic2bto/ive_been_a_nail_biter_all_my_life_and_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1ic0fno</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>really worried abt how my last gel-x left my natural nails!!</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic0fno</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1ibzeky</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Trying to track down this polish</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibwuph</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1ibz4uw</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Dupe recs for this mini polish</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibz4uw</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1ibyxm7</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Inspo needed: I never get professional gel nails, I’m an at home mani kind of gal. I’m going to treat myself, what is a gel color, style, etc that you would get that you just can’t recreate with regular nail polish?</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ibyxm7/inspo_needed_i_never_get_professional_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1icoz1z</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Press on nail set I just did</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lc1v4bqa4wfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1icck95</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Where to buy designer brand name charms for acrylic nails?</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1icck95/where_to_buy_designer_brand_name_charms_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1ico243</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Would you guys wear these press ons?</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ico243/would_you_guys_wear_these_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1icm3xq</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Year of the snake 🐍</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icm3xq</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1icl9xd</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>My husband asked for these</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8oppw1eaxufe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1ickru3</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Circuit Nails Tutorial</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3pi5sxddsufe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1icjolz</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Coquette Valentine’s cake 🎀💕</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icjolz</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1iciwk6</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Attempted tigers eye nail</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8nj85pdabufe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1ici1un</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>When do I add color to hard gel?</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5bfewps3ufe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1icgkby</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>My early Valentine’s nails. What do you guys think?</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icgkby</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1icex2v</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Squid Game</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/05ay3ybbetfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1icdrm3</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Lil fishes</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b6uvfryh5tfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1icdhg2</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Pickle nail 🥒💅</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icdhg2</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1icc0ph</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>A few of my favourite sets from last year 💅☺️</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icc0ph</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1icbg9e</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Can you use amazon gels for nail art?</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1icbg9e/can_you_use_amazon_gels_for_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1icbbgx</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>This weekend's sets :)</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icbbgx</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1icaip3</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Should I make these a set?</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icaip3</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1ic93zt</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>some random sets i’ve done while teaching myself gel x</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic93zt</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1ic82dl</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Sky nails!</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cef7xb810sfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1ic6zrw</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>My Favorite Set I Did #1</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6era23n9srfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1ic5kko</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Does Anyone Else Play Diablo 4?</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sg1sfzeyhrfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1ic58t6</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Blue or red?</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic58t6</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1ic4ylt</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Still don’t know if I like them or not</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic4ylt</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1ic4v1o</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>just made, they were going to be black but I decided to go for blue</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic4v1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1ic1yg3</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>French and psychedelic</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjpin6nxoqfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1ic1kp5</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Neon Valentines Nails 🤩 ya know I had to make them glow in the dark!</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ic1kp5</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1ibzs3g</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Galaxy nails!</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c24cc9xa3qfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1iby6s5</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Spring press ons 🌸</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iby6s5</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1ibxmfn</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Snoopy nails (sep 24)</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ibxmfn</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jan 30 08:10:16 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_02.xlsx
+++ b/data/collected_data/2025_02_02.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C715"/>
+  <dimension ref="A1:C890"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12588,6 +12588,2981 @@
         </is>
       </c>
     </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1idi1x2</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Did my own nails tonight. White chrome with unicorn</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idi1x2</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1idgh5q</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>please help!</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idgh5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1idhbf8</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>January nails</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/27p3a3y6z2ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1idgryv</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Gelx with apex?</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idgryv</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1idgg1y</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Megan Thee Stallion attending Gaurav Gupta Spring Summer 2025 Haute Couture show in Paris wearing Chakric Drape Chain Gown</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pj869ldzp2ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1idfuib</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Barbie Pink French tips</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idfuib</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1ide3v0</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Weird black marks</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ide3v0</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1idebwo</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>How many should I fix? Done by student</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idebwo</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1ideaz6</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Let's see how long the charms and gems last 😅</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/de7u6pml52ge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1ideasx</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Hybrid gel (tap) nails</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ideasx/hybrid_gel_tap_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1iddlp5</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Did I get ripped off?</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iddlp5</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1iddiio</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>My mom did my nails!</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/63f0n0psy1ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1idcbo2</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>pink french 💅✨</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7wiiranvo1ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1idc9xy</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>First real attempt at press ons!</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e69chn3ho1ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1idc3qg</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>💜Purple Galaxy Nails✨</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j6l9s4e0n1ge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1idc2j9</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Fresh new set on a ho</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bmt8oynqm1ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1idc12f</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Valentine’s nails</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ql7qwwem1ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1idc0hd</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>subtle Valentine's nails 🩷</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idc0hd</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1idbqdt</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>How to deal with press on nail that’s too small?</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0jhstz1k1ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1idbg5d</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>My floral design 🩷</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mj2kax3kh1ge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1idbeph</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>My nail journey</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idbeph</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1idbbm8</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>pictures !</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1idbbm8/pictures/</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1idb4cl</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Birthday nails 💜</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idb4cl</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1idaghl</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>can i ask for my set to be redone? mismatched and uneven</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idaghl</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1idamsv</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>I suck at painting snowflakes, so I got stamps.</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l3gqc5ana1ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1idb393</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>My first PPU order on my little shorties. A Fox in Spring Court.</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idb393</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1idao7d</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>My daughter asked me to do her nails for her winter formal this past weekend.</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58dlarsya1ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1idansp</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>So simple but probably the cutest valentine set I've ever gotten ❤️🩷💜💖</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idansp</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1idaina</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Im so proud of my natural nails😍💅🏼</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xh71sklm91ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1id9tio</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Uhmmmm, obsessed with my manicure today 🥰</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rbdrfcx641ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1id9meb</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>I did Kitsune nails today</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/59mjwrno21ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1id9e9u</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Help! Thin Nails, Allergies to Most Polishes, and Shellac Lasts a Day – What Now?</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1id9e9u/help_thin_nails_allergies_to_most_polishes_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1id9e22</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Why my nails are transparent on some spots?</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id9e22</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1id9dii</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Had to show this design off!</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/boxc16dn01ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1id961j</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Valentines nails</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eikd8dovy0ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1id91w8</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Anyone struggling with dip powder at home?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id91w8</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1id8zfc</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Tips for tying shoes with long nails</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1id8zfc/tips_for_tying_shoes_with_long_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1id8vef</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Did some jade snake nails for lunar new year</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id8vef</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1id8e1v</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Fill being the same price as a full set</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1id8e1v/fill_being_the_same_price_as_a_full_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1id6pjm</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Finally beat my cuticle biting addiction</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id6pjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1id7ftg</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>What exactly did this damage?</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id7ftg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1id7c4t</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Valentine's nails</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w8lzqxo6k0ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1id7563</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Did my nails for the first time myself 🥹</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwd4im3pi0ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1id6z2f</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Acrylics</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xhc3yr1eh0ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1id6h1w</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>dark red cat eye nails 💅🏻🐈‍⬛🤩</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b3i8iblkd0ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1id6834</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>✨ Green, Rust, and just a little Magic ✨</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id6834</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1id67nv</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Feeling in love with my Valentine set ♥️</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nm5itsgkb0ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1id5zl7</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Static Nails :/</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1id5zl7/static_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1id5r35</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Anyone know why this is happening? It’s been going on for years</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gezzb1a380ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1id5rjy</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Do these look professional?</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id5rjy</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1id4oc7</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Nail growth</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0dtd52500ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1id5b78</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Lifelong nail biter, first manicure without acrylics</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id5b78</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1id4t25</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>I want to learn nail art ass a hobby..what kind of polish should I use?</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1id4t25/i_want_to_learn_nail_art_ass_a_hobbywhat_kind_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1id4vvd</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Chrome rubbing off</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dsr52zvo10ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1id4qel</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>New almond [natural] nails with dip! Good with skin tone and hand shape?</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id4qel</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1id4gh0</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Bow Nails</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id4gh0</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1id4d3z</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Went in for basic manicure… got gel?</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n2c6zmwtxzfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1id3vu0</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>red border near top of GelX - should I be concerned?</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id3vu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1id4acs</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>RANT</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1id4acs/rant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1id41m0</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>How can make my nail area look less dry?</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hbapotoavzfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1id3xyi</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Aquarius Themed Birthday nails</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id3xyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1id3vr3</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>My hen do nails. Theme = party</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id3vr3</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1id3owx</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>What kind of manicure should I get?</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1id3owx/what_kind_of_manicure_should_i_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1id3oe9</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>AOE have tiny pinky nails?</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1id3oe9/aoe_have_tiny_pinky_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1id30pl</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Nail Injury - Matrix Keeps Coming Out</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id30pl</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1id3ihj</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Spring nails 💅🏻 🌸</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gcld0nmfrzfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1id2l64</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>This is frustrating. should I trim and start over?</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pwd9usalkzfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1id2da0</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>First time doing cateye. I’m in love!!!😍</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qqabx071jzfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1id1fsi</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Valentines nails</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vlwqnemfczfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1id0ztx</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Done some soft gel tips at home</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id0ztx</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1id0vm6</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>My husband lets me do manicure on him. 😂</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id0vm6</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1id0pxa</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>🤍 French tip</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eqixg9h87zfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1iczs0v</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>White tips &amp; gems 💅🏾</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vj9m7zdi0zfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1iczimw</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>I love this effect🥹🎀</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cuf9hlomyyfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1icz1lf</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>What to “order” when getting hard gel at salon?</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1icz1lf/what_to_order_when_getting_hard_gel_at_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1icz1ew</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Valentines Day Set</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2gd9odg6vyfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1icyvbs</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>new set👹</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icyvbs</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1icyik9</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Are these nail charms safe ?</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1icyik9/are_these_nail_charms_safe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1icygum</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Just an awesome set of nails😁</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3qbbh75ryfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1icy9v3</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>my wedding nails 🤩</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icy9v3</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1icy8w8</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Goth fairy nails</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mj9czvqjpyfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1icy8fp</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>My LNY nails :)</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfj5y6ogpyfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1icy1er</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Natural Nails</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1icy1er/natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1icxsz3</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Can I get Acrylics only for a week?  need advice</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1icxsz3/can_i_get_acrylics_only_for_a_week_need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1icx1gi</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Big brain beauties, help me figure out if I may have a HEMA allergy?</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1icx1gi/big_brain_beauties_help_me_figure_out_if_i_may/</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1icx1z0</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Which nail shape should I get?</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icx1z0</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1icuf5w</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>What is this discoloration</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icuf5w</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1icwv09</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Gel nails going dull, can I put clear varnish on top?</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1icwv09/gel_nails_going_dull_can_i_put_clear_varnish_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1icvql7</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Beetles Polish and Fake Nails</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1icvql7/beetles_polish_and_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1icv6wy</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>What shape is this?</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icv6wy</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1icskps</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>the cutest nails ever by @cutiecles.byjade on instagram</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84pl822lexfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1icwxoe</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>nails for valentine’s day 💖✨🌷</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icwxoe</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1icwxg9</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>What brand of full cover nail tips have SUPER small sizes. These companies *cough cough* apres *cough* made these bigger sizes but I need really narrow ones. My pinky is 0.23 inches of 0.58 mm. And yes I can file it, but try holding a super tiny nail tip and filing it... it's very difficult lol.</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1icwxg9/what_brand_of_full_cover_nail_tips_have_super/</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1icwi4b</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Early Valentine’s Set</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icwi4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1ict98a</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Born Pretty</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ict98a/born_pretty/</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1icw220</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Ditsy Valentine 💐💕</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7kf8s7k89yfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1icux6s</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>What do you think about my new nails?</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nx5b4kv90yfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1icuvje</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>My Valentine’s Day nails 🥰🩷</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icuvje</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1icuead</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>This is such a pretty colour, I can't</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dyhdq03xvxfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1ictrtq</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Trans pride nails!!</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i39n7exdqxfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1idi6eg</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>My extremely messy crappy valentines nails</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idi6eg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1idgz2k</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Do you have to get gel filled or can you shellac?</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1idgz2k/do_you_have_to_get_gel_filled_or_can_you_shellac/</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1idgv74</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Anyone tried Pop &amp; Polished crackle?</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1idgv74/anyone_tried_pop_polished_crackle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1idfjdc</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Pretty, pretty good</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idfjdc</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1ideldj</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>LynB Be Chill My Beating Heart</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ideldj</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1ide269</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>From design to reality: Happy Chinese New Year! 新年快樂! 🧧🎊</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ide269</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1idcshi</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Mooncat Plankton vs Cracked Boujee Emerald Swatches</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1idcshi/mooncat_plankton_vs_cracked_boujee_emerald/</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1idcqpf</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Polish brands you will never buy because of their branding or packaging?</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1idcqpf/polish_brands_you_will_never_buy_because_of_their/</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1idc8pn</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Happy Lunar New Year!</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idc8pn</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1idbewb</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Please help me find a dupe for Sally Hansen Fairy tale Ivory</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idbewb</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1idauus</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Colores De Carol- Venetian Majesty  | PPU Jan2025</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idauus</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1idapcx</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Happy Lunar New Year 🧧🐍</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idapcx</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1idaowi</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>pt. 2/2 of all my blue lacquers, swatched! All cremes this time, except for the ones that aren’t 💙</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idaowi</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1idajss</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Alchemy Lacquer- Venetian Opulence | PPU Jan2025</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idajss</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1idahnf</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Phoenix Indie - Optical Blast 💛🩶💙</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g207c23e91ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1ida2y4</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>january’s nails 💅</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ida2y4</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1id9ruh</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Polished For Days Eternal Glow + Catch My Drift</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9l1mq5u31ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1id98rr</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>sabertooth ✨</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id98rr</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1id95qi</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>First Magnetized Mani</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id95qi</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1id8ses</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>a fox in the spring court ✨🦊🍃</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rhtf9bunv0ge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1id8pmk</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Trying to decide if I like this color</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id8pmk</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1id6g4m</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Ok I get the Deep Space hype now</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rptkfo9dd0ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1id6amn</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>The only color I’ve been wearing for the past three months.. Bubbles Only! 🫧❤️</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/im0qf2g7c0ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1id67tu</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>MoYou London closing their US site? :(</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vu8cr9ylb0ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1id5p8n</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>✨ Green, Rust, and just a little Magic ✨</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id5p8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1id5ibg</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Really loving this color</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id5ibg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1id5b6n</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Nail from the last months</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id5b6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1id4y3i</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Did OPI RapiDry Spray get discontinued?</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1id4y3i/did_opi_rapidry_spray_get_discontinued/</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1id4is0</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>finally got to try deep space!!</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id4is0</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1id4io9</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Mooncat After the Rain💜🧡</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id4io9</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1id3mjw</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Magnetics are going to take over my life</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rhvcizy9szfe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1id3h9v</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Post service woes</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1id3h9v/post_service_woes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1id2rjm</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Magnetic magic ✨</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/km3he62slzfe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1id1vpd</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>trying to find a good green</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id1vpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1id1jl5</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>I have slept on Everything Taco</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id1jl5</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1id1d55</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Lurid's I Love You Always</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id1d55</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1id16od</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Thick - Strong Top Coat needed for brittle nails!</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1id16od/thick_strong_top_coat_needed_for_brittle_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1id0xa3</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Cirque Lucky Bag cost last year?</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1id0xa3/cirque_lucky_bag_cost_last_year/</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1id0uib</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Olive and June cremes</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1id0uib/olive_and_june_cremes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1id0sxq</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer - A Fox in the Spring Court</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id0sxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1id0npm</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Secrets and Scandals</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id0npm</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1id0lca</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Is ILNP Shapeshifter warm?</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1id0lca/is_ilnp_shapeshifter_warm/</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1id0hon</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Aquarium Nails</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id0hon</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1icytkf</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Nails change shape when painted?</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icytkf</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1icyeoi</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Those of you who paint press-ons with normal lacquer, what brand do you use?</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1icyeoi/those_of_you_who_paint_pressons_with_normal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1icy2rp</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>✨️🌈Pastel Linears🌈✨️</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icy2rp</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1icxv1q</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Nails Inc mani 😍</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icxv1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1icwra4</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>My first French mani 💅</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x45tn5jmeyfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1icw2t2</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Fairy sparkles</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/37dst56g9yfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1icuys0</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Lunar new year mani 🐍</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icuys0</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1icuphi</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Im always SO blown away by the sparkle in Holo Tacos Menchie The Cat 😻</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nq23o2o9yxfe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1icujzu</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Tiny bubbles in polish?</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icujzu</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1icu2qj</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Trippy AF</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qjsaxbyysxfe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1ictp4f</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>In love with my nails now</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ictp4f/in_love_with_my_nails_now/</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1icsk19</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>New collection alert</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1icsk19/new_collection_alert/</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1icdtbk</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>dupe for essie smooth-e?</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1icdtbk/dupe_for_essie_smoothe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1icgjib</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>So sad &amp; bummed</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1icgjib/so_sad_bummed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1icrfaj</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Back with my 4th annual Lunar New Year nail art: Year of the Snake 🐍🍊🥟🎆🧧</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icrfaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1icpizx</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>How can I prevent this from happening?</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rydtk0j3cwfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1idfafd</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>V-Day Nails!</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idfafd</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1iddnra</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>A lil DIY mag gel ☺️</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/od6t93f002ge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1idd3p2</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Valentine baddie vibes</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idd3p2</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1id9pwc</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Valentines Day Inspo</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5s3bsceg31ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1id90z3</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Did these vacation nails😩</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcdoo6cox0ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1id8pv7</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>CNY nails! Really happy with how they came out, especially the hand painted details 🐍🧧 Swipe for close ups!</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id8pv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1id8nb3</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>First Press On Set for my Sister's Bday!</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zzmlv3ymu0ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1id83jg</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Critter nails 🐛 🐸 🍄</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ubn51p5q0ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1id74sp</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Heart cat eye nails! Took over a week to get the right technique</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dqz036dmi0ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1id68dp</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Earthy Inspired Polygel Nails</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8yll381qb0ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1id41kp</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Went to make Valentines day nails ended up with Christmas nails 🫠🫠</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id41kp</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1id0a5s</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Valentines nails 💅</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id0a5s</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1ictkst</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Cat eye Beating Hearts for Valentine’s Day! 💗💗</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/paz36jcmoxfe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1icquuk</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>New chrome nails</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1icquuk</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1icq8yg</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>what do we think the technique was?</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vhhvz4q3mwfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1icpe07</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Geles ojo de gato</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1icpe07/geles_ojo_de_gato/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jan 31 08:10:23 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_02.xlsx
+++ b/data/collected_data/2025_02_02.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C890"/>
+  <dimension ref="A1:C1093"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15563,6 +15563,3457 @@
         </is>
       </c>
     </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1ie9mqu</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>My new manicure looks perfect</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvxp2h7t8age1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1ie9fwn</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Found the most gorgeous nude for me!</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hdcupotc6age1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1ie96cx</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q86mx1ew2age1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1ie8soh</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Posting my January nails on the last day of January ...</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xcguhx83y9ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1ie8i27</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>I like thiw color tho.</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qr9i410eu9ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1ie8erm</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Cat eye ombre nails with glitter tips 🐱</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84vpu9rbt9ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1ie8ch9</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Dominant Hand Thumb Press On Keeps Popping Off?</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ie8ch9/dominant_hand_thumb_press_on_keeps_popping_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1ie7q9u</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>the second set i’ve made :D</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9l993d2ml9ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1ie7efq</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>December nails…my natural nails</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xwpg4w1i9ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1ie74g4</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Let me know what you think!</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iaaxwby6f9ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1ie70z9</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Are these horrendous or not BE HONEST</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/grrwevv3e9ge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1ie6wca</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>French for the win!</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/14ng2z4vc9ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1ie12qn</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>So maybe not acrylics, what else or just a break?</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/59lqmtc0w7ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1ie65l2</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>what is this…</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rw175a0e59ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1ie5y5b</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>New set for my first day at a new job on Monday</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7irev2db39ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1ie5ryo</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Love my Valentine’s nails 🥰🩷</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8mk7zkgm19ge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1ie5o8r</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Nail curve</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wv9q7h7n09ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1ie5nnf</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>When I learned how to do una gella nails and chrome</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9fymq5kh09ge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1ie2x2m</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Clase Azul Inspo Nails</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie2x2m</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1ie5myi</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>What should I be asking for if I need these done ? It doesn't look like regular gel polish to me...it's almost translucent and dreamy 😍</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/abjwp4xa09ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1ie4xte</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Gel? Dip? Natural nail struggles.</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ie4xte/gel_dip_natural_nail_struggles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1ie5exp</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>CNY nails 🧧🐍🪭 Super proud of the results 🥰</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie5exp</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1ie4lra</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Is it too obvious that this is press on?</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6nq738rhq8ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1ie4h49</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Valentine's Day nails</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gg59x5cbp8ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1ie4fql</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>I love my nails and this is only 15$ !!!!!!</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o8fgabdlo8ge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1ie3v2w</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>What should I do?</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ie3v2w/what_should_i_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1ie3nwc</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>What did I do wrong?</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ie3nwc/what_did_i_do_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1idxwre</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Nailtek</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1idxwre/nailtek/</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1idxs02</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Question About Different Polish Types</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1idxs02/question_about_different_polish_types/</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1ie33r2</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Should fills/rebalance cost less than the original overlay?</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ie33r2/should_fillsrebalance_cost_less_than_the_original/</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1ie2szv</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Leopard nails</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ocr9xipa8ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1ie2swd</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Gold and Pearls 😍 my nail tech did her big one ✨</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie2swd</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1ie2lb7</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>I am so back. This is my first set of Acrylics after experiencing contact dematitis with gel.</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie2lb7</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1ie2elx</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Recommendations for noobie?</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ie2elx/recommendations_for_noobie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1ie27dq</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Transparent part of nails?</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/freiae2i58ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1ie1xrj</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Valentine’s Day/Lunar New Year Nails 🩷🧧</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie1xrj</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1ie18mt</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Choosing nail shape</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b2qymk4dx7ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1ie16mr</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>V-Day set💋</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cvqui8eww7ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1ie0gbl</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>basic but so am I</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jp2vn5rwq7ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1ie07rj</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Polish over press on nails</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kn8gyss2p7ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1ie02mw</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Which nail shape suits my hands best?</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie02mw</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1idzycq</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Cake Nails</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idzycq</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1idznmz</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>my valentine’s set 😍</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idznmz</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1idzkvv</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>birthday chrome!</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okxyfnb4k7ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1idz857</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>rat nails!! 🐀🧀</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mbiahw0hh7ge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1idyqod</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>❤️💛 Lunar New Year nails</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vp1f21osd7ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1idyhuk</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Few nails I got done for the past years</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idyhuk</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1idy7w4</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Got a compliment on these lil ladies today.</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8uvwckt97ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1idxz1h</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Colors that go with green emerald ring 😊</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1idxz1h/colors_that_go_with_green_emerald_ring/</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1idxmj8</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>[OC]first time doing acrygel, give me tips to improve!</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idxmj8</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1idxfkx</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>My art VS inspo pic! Inspo from @September elm秋榆 on Rednote! Also a question regarding starting out.</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idxfkx</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1idx7x0</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Growing fast or not close to the cuticles? Got on January 20th and it’s the 30th. Worth doing again?</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idx7x0</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1idwv5o</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>gel polish</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1idwv5o/gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1idw3t0</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>How do we feel about white base cat eyes?</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m3o0wr5ut6ge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1idwrtg</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Nails by B.M.E. Nails :) a local nail artist where I live. Thought they were super pretty</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxzlu6qxy6ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1idwntq</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>I guess it’s time for a trim 🥲</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bn2shab4y6ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1idvu2r</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Least damaging to my nails</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1idvu2r/least_damaging_to_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1idwavr</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Are press ons allowed?</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dr2l9ez9v6ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1idw1l5</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>my wicked nails!!💚🩷</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3t8kzamft6ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1idvrrz</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Nails by Kismet Claws, thought they were cute and wanted to share</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idvrrz</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1idvp4t</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>How to ask my nail tech…</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1idvp4t/how_to_ask_my_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1idvdlf</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>🍒♥️ Yay or nay? Using 3 acrylic colors</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idvdlf</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1idv7vs</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Started taking care of and trying to grow my nails since November 2024 .</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7v05avbn6ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1idv2ly</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>IBD gel different that biogel?</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1idv2ly/ibd_gel_different_that_biogel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1idv1oq</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Gel X doesn’t stay on my nails</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1idv1oq/gel_x_doesnt_stay_on_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1idv1fz</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Russian Manicure/builder gel</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1idv1fz/russian_manicurebuilder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1idu235</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>first time my natural nails, I try to leave acrylic permanently</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s6gjjyxte6ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1idtxbo</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>How would I ask to get my nails done like this?</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/av4t80ltd6ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1idts96</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>BTartbox nails</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xhe3vzakc6ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1idtqmw</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Red pedi</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idtqmw</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1idsw1r</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>❤️✨ valentines nails (and cat)</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7n53ojb566ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1idsb5t</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Skin under nails extremely dry since I got acrylics</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n9sd9nqv16ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1idro4l</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Giving Sue vibes from "The Substance"</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idro4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1idrjyp</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>How do you feel about summer sets in winter?</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idrjyp</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1idsqft</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Do I have ring of fire? ☹️</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3swv5bi056ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1idsojr</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Birthday nails!</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l5argxrm46ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1idryz1</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>No you don’t understand, I’m obsessed.</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f03cadpez5ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1idrqul</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>❤️💋</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idrqul</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1idrhvt</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Is there anyway that I can preserve a set of nails I got?</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4vhpodxv5ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1idr9a7</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Art work!</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mmrb3gy4u5ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1idkd8r</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>How to heal!?</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idkd8r</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1idkecy</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>press on gellack nails?</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1idkecy/press_on_gellack_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1idnhxk</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Color identification help needed! Inspo from Carrie Summers on Pinterest!</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g6tbe3gyz4ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1idqhpl</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Growing out my nails, advice on Caring for them</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rnc1z0oco5ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1idqd2v</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Tried something new and I’m so divided. Is it pretty or bad?</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wrwyl5edn5ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1idq307</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>i went outside &amp; it was warm.</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uvmtieh8l5ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1idpz8u</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>How long do you carry out maintenance?</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ox3sxw4fk5ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1idpnag</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>i loveee experimenting with layering chromes and cat eyes</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hkafu8oph5ge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1idpjd1</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Gel nails question</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1idpjd1/gel_nails_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1idouge</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>one of the trending designs for 2025 girls! Double French!</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kd9l7lmeb5ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1idok8t</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>A nice option to show off blue 🩵</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngfgyjo095ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1idofpb</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Trying on press on nails</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1erzlb0z75ge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1idoav1</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Got Gel x for a wedding and I hate the design - I’m thinking of doing a soak off and just another simple set in 2 days to fix it, is this too soon?</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1idoav1/got_gel_x_for_a_wedding_and_i_hate_the_design_im/</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1ido4g1</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Yall…help a friend please lol</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ido4g1/yallhelp_a_friend_please_lol/</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1idmu3f</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Good job</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5vws28ztt4ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1idmtxo</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Booked in for a nail appointment, can I get acrylics with these?</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rt2hyryxt4ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1idm7ok</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>cat eye nails</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggetm21yn4ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1idlfoc</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>🩷 My second tribute to the month of love 🩷</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p47tp10of4ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1idla3w</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>How to create a coffin shape for short nails</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ujcpm9yd4ge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1idl80f</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>blue addiction</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qgs84j2ad4ge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1ie968d</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Is it just me or is kbshimmer very heavy on the fumes</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ie968d/is_it_just_me_or_is_kbshimmer_very_heavy_on_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1ie8qqz</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>No need to cry over Mercury’s Tears</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8ccnwlodx9ge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1ie8mvs</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Fields of Lavender 💜❤️</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie8mvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1ie7ecm</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>which combo for my next mani? 👀</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie7ecm</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1ie72pf</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Jan 2025 - Aug 2024</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie72pf</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1ie6mxb</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Haven’t done my nails for over a year but it feels great getting back into it!</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j9ly1i54a9ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1ie6kep</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>OPI must be taking cues from indies, their spring collection is full of shimmers and flakies!</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dhcmnt4f99ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1ie6g2a</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Is it normal to be brand new &amp; less than 1/2 full</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23bnitj789ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1ie5tbg</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>I Thought I'd Like This More</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8rp082j029ge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1ie5js1</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>5 Minutes before I snapped the middle one</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9zz724gez8ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1ie57xs</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>How do you decide what polish to wear?</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ie57xs/how_do_you_decide_what_polish_to_wear/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1ie4ze1</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Please help me decide which Emily de Molly to buy for my birthday. I must eliminate 1.</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fr0vysn3u8ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1ie4rpu</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>My first share here - a Lunar New Year mani in Pantone color of the year mocha mousse 🤎</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie4q63</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1ie3weg</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>{PR} Lunar New Year Nails</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie3weg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1ie3d1c</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Tried a $2 galaxy polish…</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie3d1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1ie3bn3</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Zoya Sophia for Lunar New Year</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie3bn3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1ie2pib</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>My first skittle mani!</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie2pib</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1ie258s</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Happy Late Lunar New Years</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie258s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1ie1cef</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Fun colors to soothe the pain of the big chop</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6tc6c29y7ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1ie19eb</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Made use of my ILNP Magnet</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie19eb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1ie1615</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Thought I’d step out of my comfort zone but I’m unsure how I feel about these</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/macerm5jw7ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1ie101k</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Chúc Mừng Năm Mới! (&amp; help with stickers?!)</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie101k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1ie0oge</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Day 1 of 14 days of Valentines nail inspo 💕 a shooting star moment</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie0oge</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1ie0o2c</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Best blue polish I own</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie0o2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1idzds2</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Thermal nail polish history</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1idzds2/thermal_nail_polish_history/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1idzp9f</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>😐</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9f7n0y4l7ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1idzmzr</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>year of the snake mani 🐍</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/azq0q8qmk7ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1idxbrp</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Pinterest inspired nails</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/faom2hp537ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1idypfy</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>❤️💛 Lunar New Year nails</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b1mqkk8jd7ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1idxos6</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Storing Polish on its side?</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1idxos6/storing_polish_on_its_side/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1idx2kx</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Has anyone used Essie To the Rescue?</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idx2kx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1idwkyu</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>why does my nail polish always peel like this</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idwkyu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1idw8m9</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Essie topcoats - no chips ahead and gel couture?</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1idw8m9/essie_topcoats_no_chips_ahead_and_gel_couture/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1idw16p</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>How much is too much? Is there such a thing as too much?</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1idw16p/how_much_is_too_much_is_there_such_a_thing_as_too/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1idvv4i</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Reflection Pool</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idvv4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1idvjl8</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>When do moisturize and give your nails a break?  Does this nail look dry?</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ssbkbqrp6ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1idviws</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Be am careful who you give your information to…especially right now</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1idviws/be_am_careful_who_you_give_your_information/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1idv4tx</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Trying New Shimmers</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/92pqstnpm6ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1iduz4b</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Give me one honest thing - bkl</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iduz4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1iduwml</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>SOUND ON for full experience 🪐</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xu6476i1l6ge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1idudg6</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>By Vanessa Molina- Midnight Masquerade | PPU Jan2025</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idudg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1idu4ch</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>new years nails 🧧❤️</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idu4ch</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1idu24t</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Fair is Ferragamo</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1idu24t/fair_is_ferragamo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1idtud3</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Intense Bioluminescence with Starlight underneath</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bdez8ck6d6ge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1idtgtk</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Tip wear solution - FA at color blocking</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idtgtk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1idtg09</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Secrets and Scandals</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idtg09</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1idtcn3</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Mixed feelings on this one</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8h2yfd6h96ge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1idt0mc</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Glacier Glow :)</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idt0mc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1idszac</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Rainbows n Critters</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vhm2l3ht66ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1idsqb8</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Mood: GTFO My Uterus</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idsqb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1idshjy</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Get Off My Tail 🧜</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g3enbx9x26ge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1idsftc</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>A month in polish! ❄️</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idsftc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1idsfri</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Happy Lunar New Year 🐍</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idsfri</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1idrsrh</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Teddy</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xqzc8o45y5ge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1idr7wq</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Mooncat - Ultrahot</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kgj712lut5ge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1idqj5o</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Lunar New Year nails with ILNP opal sunset as a topper</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idqj5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1idq2hw</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Sassy Sauce Blowin Bubbles</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idq2hw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1idpz3i</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Velvet Teddy 🧸</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/137jywvdk5ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1idps7i</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Forever matching my nails to my plants 🌿</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k3cdhe1si5ge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1idps7f</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>It just felt right today 🤍</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idps7f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1idp3c7</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>BKL 🍋</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idp3c7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1idp0gg</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Bugs &amp; Beetles 🪲</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idp0gg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1idos70</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Glowing on a cold morning!</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idos70</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1ido7rn</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Any tips for a first time magnetic polish user? 👀🧲</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lakcaxv265ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1ido66d</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Is this nail polish remover gone?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9qhzwrp55ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1idnpzu</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Cirque Colors - Bitchin</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idnpzu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1idngu0</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>I need to find a way to block “green shimmer lacquer” from my credit cards ASAP</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/min9pgfoz4ge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1idnf6b</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Still short but my first attempt at almond shape after 20+ years of biting and 5+ years of healing</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ft7s24raz4ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1idkm3a</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>I wasn't sure about this in the bottle but I think I quite like it!</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m0sjkzkt54ge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1icyjvf</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>the cashier at my favorite coffee shop and i wearing jewel beetle!</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rcuvmzvqryfe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1id3add</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Chrome nails no powder?!</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id3add</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1id3o2u</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>I've always been told I have big hands, what nail shape should I get that's flattering?</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1id3o2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1idh01g</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Hey heyy does anyone have any recommendations for duping this loveliness? I'm in Australia so would love some recommendations available in Australia</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcaph5fuv2ge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1idhih7</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>I am struggling so much with growing out my nails</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1idhih7/i_am_struggling_so_much_with_growing_out_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1idiwb3</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Glisten &amp; Glow Shh…Secret Crushes.</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idiwb3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1idil8d</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Dimethacrylate in regular nail polish?</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ja3tras3e3ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1ie9mu5</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>I need major help😭😭</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ie9mu5/i_need_major_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1ie8g7j</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Despite the dark knuckles rate my first nail work. its just simple i'm scared of posting it.</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ht3zr8it9ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1ie8cid</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Just my simple nail design.</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/298eq20fs9ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1ie82k0</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Inspired</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izyh57xfp9ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1ie7rkp</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>my second set :))</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhzcp0f0m9ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1ie7r95</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Cat eye gradients</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yn9hq3zwl9ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1ie7oku</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Best gel for nailart?</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie7oku</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1ie7e7m</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Can you let me know what you think about these?</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24uzjsjzh9ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1ie61gh</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Not the best but am getting better I think</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie61gh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1ie4yfu</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>My first share here - a Lunar New Year mani in Pantone color of the year Mocha Mousse</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie4yfu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1ie28r8</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>First attempt at pop art nails.</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/en7vb6vt58ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1ie16z6</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>thoughts?</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie16z6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1ie0jfb</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Laced Crystal cateye nails</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ie0jfb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1idzu3l</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Cake Nails</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idzu3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1idzpxv</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Some Valentine nails I created ☺️ 💕</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idzpxv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1idwbny</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Embossed colours and flowers</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ewfy87iv6ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1idv3xe</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Decided to try something new ! Done by me!</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0tibfntim6ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1idu524</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Valentine manicure</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x0tr6jggf6ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1idtsnw</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>New set 🩶 - how did I do?</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nyjzxabuc6ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1idtpu1</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Red pedi</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idtpu1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1ido65z</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Isolated Chrome + Cat Eye ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8mxhoop55ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1idqg3w</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Mew inspired nail’s</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idqg3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1idpxvg</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Y2K Nails</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mfhqcht3k5ge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1ido3vl</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Valentines nails!💖</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ido3vl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1idnn2a</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>First snakies!</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idnn2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1idm9zr</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>I’m so in love with the stained glass nail art trend at the moment 😍</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idm9zr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1idl4an</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>I feel prettier and happier at work when I have new nails 😍</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1idl4an</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Feb  1 08:09:20 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_02.xlsx
+++ b/data/collected_data/2025_02_02.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1093"/>
+  <dimension ref="A1:C1308"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19014,6 +19014,3661 @@
         </is>
       </c>
     </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1if1ne0</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Chinese New Year nails 🐍</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if1ne0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1if1mvw</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Chinese New Year nails 🐍</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if1mvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1if1b8s</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Is this bad?</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/otzs951aehge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1if1ame</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>One of my favorite colors ❤️</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if1ame</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1if14i6</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Has anyone ordered nail polish from NowInSeoul?</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1if14i6/has_anyone_ordered_nail_polish_from_nowinseoul/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1if0reo</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Gotta love the sparkles!</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wfqteosa7hge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1if0pg0</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>I’m obsessed with my fluffy nails</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if0pg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1if0efv</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Do these square-ish nails suit me or should I try a different shape?</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if0efv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1if07r2</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Valentines nails💋</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if07r2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1if07jd</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Got my nails done for my birthday &lt;3</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if07jd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1iezc6p</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Inspo: @mabelandrowe on insta - people pleaser nail lover</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lzefy87eqgge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1iezn2i</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>BKL Lemon is divine.</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nvx4a59stgge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1ieziiv</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Heart and pearls ✨️</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ntm34dpcsgge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1iezfor</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>pink with black ribbon nails 🖤🎀</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jo04amzgrgge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1ieyy78</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>I wanna keep my nails strong and pretty without getting them done!! How??</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ieyy78/i_wanna_keep_my_nails_strong_and_pretty_without/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1ieyvqc</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Do my nail beds look freaky?</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0n4uywflgge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1ieysak</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>🧼🍬🛼🧬🫧loving the way these came out! 🎀</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ieysak</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1ieyasc</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Wasn’t sure about the combo at first but I feel like a winter witch</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y0yh5wj3fgge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1iey253</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>New Nails</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ypqafnvncgge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1iexjcs</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Vday Press Ons</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iexjcs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1iexiq8</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>My nails 😊</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4pouqkkb7gge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1iexegi</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Since y’all hated the gray…</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iexegi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1iexcqy</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Valentine’s ready 🎀</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1m2ccyxo5gge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1iex2j0</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ee1h4rjv2gge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1ievvgg</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Nail wraps/gel stickers (ex. Dashing Diva) experience??!</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ievvgg/nail_wrapsgel_stickers_ex_dashing_diva_experience/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1iew5ji</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>is there anyway to disguise this?</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iew5ji</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1iewlfb</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>New Set by Me</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tv8ojv5dyfge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1iewjf2</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Back to my natural nails!</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hz7357itxfge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1iewiv8</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Anyone know black nail polishes that are really sleek and shiny that make your nails look like this</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iewiv8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1ievq79</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Valentine’s Day - but make it dark</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5i0q9fe3qfge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1ievpa9</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Is this a good starter kit for personal use? Open to any suggestions ☺️💌</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ievpa9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1ievld1</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Aurora Borealis</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zpfvp9nsofge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1ievgkp</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Valentines nail set ^.^</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ht04k0zlnfge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1ieutzl</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Does anyone know why this happens?</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ieutzl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1iev63f</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Forbidden Fruit Colours!!</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iev63f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1ieuyjq</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>A lot of colors 🌈</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/57ipvlezifge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1ieuojy</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>I'm obsessed with this set 😍🖤</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56gqld8hgfge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1ieuk8s</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Dvok New Moon Collection</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ieuk8s/dvok_new_moon_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1ieu4py</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Can I cover my nails with regular polish?</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ieu4py/can_i_cover_my_nails_with_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1ieu3yk</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>First gel set! 🌸🩷</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ieu3yk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1ieu0wj</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>How did I do?</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/djx3cnpsafge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1ieu0u0</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Did my nails today, I think they look so fun 😋</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ieu0u0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1ieu0fp</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>First decent set I’ve done!</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/30cc10hoafge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1ietqno</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Miffy nails!</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ietqno</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1ietpgn</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>It’s giving Barbie 🖤</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jkft19638fge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1ietp3j</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Valentines but not VALENTINES nails 🌸</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0wxabzz7fge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1iet9o7</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Need more apex but getting closer</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iet9o7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1ietfk1</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Doing my Nails again after having Breast Cancer 🥳💅</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1cbrvc3s5fge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1ietjzz</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Strengthening natural nails</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ietjzz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1ietg9h</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>strawbs... my nail tech is so cool</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ietg9h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1ietau4</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Did my own Gel X set🩰</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9m7gx6q4fge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1iet3c5</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Valentines day nails</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iet3c5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1iet06a</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Saw this color with the glitter and then i was in love with it 💞 def a good choice ☺️</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/siuya4na2fge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1iesxeb</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>February Nails</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1x243ehn1fge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1ieswsq</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Wanted to share my nails from October (my fav season)🎃</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czb69dki1fge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1iesc3m</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>fav sets of all time</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iesc3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1iesd14</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>My Grateful Dead Mani with waterslide decals I printed.</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d1bryjozwege1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1ies6ds</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Butterflies and carefree vibes</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ies6ds</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1iery9g</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Early V-Day 😌</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1vqd8hrtege1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1iermff</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Red 80s vibe!</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r7ddex05rege1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1ierbv3</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Tried a different shape🥰</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ierbv3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1ierbio</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Slowly breaking nail</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ierbio</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1ier7nv</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Natural nail victory!</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ee3higkunege1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1ieqvvf</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>V-day mani 💒 My nails are so thin it’s only a matter of time before these split. I’m glad I took a nice photo before they do</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lv9yan3clege1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1ieqtvb</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>My attempt on Valentines Day nails 🤗</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ieqtvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1ieql4w</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>let my nail tech do her thing 💫✨</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ieql4w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1ieqdsc</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>What is causing this lifting?</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ieqdsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1iepywr</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>3 weeks of growth and looking so much better!</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iepywr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1ieqbau</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>cute valentines nails ♥️</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/72v5nib0hege1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1ieq2k3</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>primark nails</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ieq2k3/primark_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1iepvyh</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Best "gel-looking" nail polish?</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iepvyh/best_gellooking_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1iepm3q</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>How do I even fix this?</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/38zldw5obege1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1iepjhc</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Totally obsessed</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8lkhatb4bege1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1iepidh</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Oh hey I have a question: how will I ever get anything other than cat eye nails after this??</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iepidh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1iepg7x</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Listas 😍 que opinas? Las amo demasiado</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4h8kjpsfaege1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1iepfvz</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Subtle Valentine's Day Set 💕</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hga2ou5daege1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1ieoqv6</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Recovering nail biter</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vd0ytsk45ege1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1ieonoq</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Please convince me these aren’t as horrible as I think❤️‍🩹I usually do almond, long and a neutral pink but wanted to change it up and absolutely hate them. I also wanted more of cherry wine color but the girl couldn’t suggest anything so these up with this brick red.</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ieonoq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1ieol62</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Worm nails</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ieol62</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1ieo8wx</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Nail strips</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ieo8wx/nail_strips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1ienxbl</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Hearts on my nails for Valentine’s ❤️💅 What do you think?</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ienxbl/hearts_on_my_nails_for_valentines_what_do_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1ienugc</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>did my own nails last night!</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ienugc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1ienrkg</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>No valentines yet, still in cute winter mode</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ienrkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1ienn2c</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>First time getting cat eye nails</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oj675tcrwdge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1ienlb9</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>New Valentine's day minimalist nails!</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xtds1t3dwdge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1ien7uq</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>My favorite nail oil</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://seranova.store/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1ien38k</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Nails Ready For Six Nations</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0p13ok6ksdge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1iemzjf</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Red cat eye (during Christmas season)</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1wldiporrdge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1iemyqq</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Goth nails 🖤🖤🖤</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iemyqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1iemswa</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>I work in a deli - any way to keep my nails from shredding and bending?</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iemswa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1ielsdb</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Nails that I did myself a few years ago. The mold cutting process drove me crazy, haha! But I loved these nails. What do you think of them?</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jkzfmuhwidge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1iem9xt</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Trying a new nail shape with hand-painted frenchies 💜💅🏼</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0sqnmnfkmdge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1iem2f7</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>First time getting my nails done</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5t2ggmlzkdge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1iem0q9</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>These are my nails</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/spwntbvmkdge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1ielzbv</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Is it common in your city for nail salons to use sterilized tools for each client?</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kh50x7eckdge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1ielnrn</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Inspired by the scaled and icy album by twenty one pilots!!</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ielnrn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1iekrlg</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Is baby oil good for nails?</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iekrlg/is_baby_oil_good_for_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1iekmxu</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>❤️</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cxo4egmgadge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1iekixl</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>🦇Almond gelx set🦇</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iekixl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1iekah1</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Chrome powder</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iekah1/chrome_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1if1aef</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Mooncat vs ILNP</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1if1aef/mooncat_vs_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1if19ii</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Seeking opaque nude for base coat</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1if19ii/seeking_opaque_nude_for_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1if0hh8</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>My favourite colour scheme</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if0hh8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1iezi4g</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Pride and Prejudice (w/ bonus comparison!)</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ky3jbr38sgge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1ieyk0k</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>update: went with ILNP fairy dust + clover combo 🌝</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zczchguvhgge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1ieygd5</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Illusionist</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fkhsgjwtggge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1ieydu0</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>the warm state does not quite match "it's brittney beach" help me find what would!</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ieydu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1iey2zc</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>January nails!</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iey2zc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1iexzrp</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>i’m a little late, but lunar new year nails 🐍</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iexzrp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1iexndu</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Mardi Gras Masquerade ✨💚</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ptkei4uk8gge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1iexapy</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Fair Isle really is that girl</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iexapy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1iex7le</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>2024 Manis</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iex7le</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1iewykb</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>I 💙 KBShimmer</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xswpkwau1gge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1iewqvt</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>January roundup</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iewqvt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1iewk06</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Dupe for gitti 004?</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iewk06</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1iewejo</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>What are your love-hate nail polishes?</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lcbcic4hwfge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1iewc05</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Best base and top coat for person who has their hands in water a lot ( artist who hand washes A LOT. )</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iewc05/best_base_and_top_coat_for_person_who_has_their/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1ievvcg</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>OPI Makeout Side DUPE</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ievvcg/opi_makeout_side_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1ievsxf</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>So shifty ✨💖✨</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ievsxf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1iev8ir</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>I love my nails today :)</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iev8ir</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1ieuueh</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Sweetheart Polish Replacement Brush</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ieuueh/sweetheart_polish_replacement_brush/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1ieuu6b</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Dupe for Chanel giallo napoli?</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gtjde69whfge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1ietaln</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Skittle of my new to me haul. All Halo Taco, one coat, no top coat. Just for fun and not really well done, but I am so excited!</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ietaln/skittle_of_my_new_to_me_haul_all_halo_taco_one/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1iet9x1</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Latex base around nails</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iet9x1/latex_base_around_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1iet3h0</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>When you are trying to create some new shades using what you have (love Mystic Haze btw 🩵🤍）</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7r29fz313fge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1iesv9y</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Dupe for O&amp;J CCT?</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iesv9y/dupe_for_oj_cct/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1ies1wu</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>A bit disappointed...</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ies1wu/a_bit_disappointed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1ieryjy</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>How I now do warm oil soaks to waste little to no precious oil</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ieryjy/how_i_now_do_warm_oil_soaks_to_waste_little_to_no/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1iernkw</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>team thermal. all hail, the ephemeral.</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iernkw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1ierjzj</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Thermal polish, my beloved</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ierjzj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1ierirc</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Monarch Butterfly Nails 🦋</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ierirc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1ieravx</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Cracked - vintage lampshade</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ieravx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1ier90p</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>ILNP - Off the Grid</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s22hr3s5oege1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1ieqhmj</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer - Sunset Over the Suburbs</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1s0q0b7iege1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1ieqffk</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>I wore so many different colors in January 😌 (and some from December)</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ieqffk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1ieqdcl</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Ilnp magnet magic</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4xksdcefhege1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1ieqa1g</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Holo taco - rose gold flake taco</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y7ixak2rgege1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1iep3or</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Cirque Colors real talk</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iep3or/cirque_colors_real_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1iep1ww</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Linear holo pinks to match my holo tamagotchi~</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xyfxlg7h7ege1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1ieof3o</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>R I fucking P</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ieof3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1ienueh</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Finally got a chance to wear this shifty classic: LynB Designs “Fair Isle”!</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ienueh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1ien7l3</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Does anyone have a polish recommendation that looks like a Japanese beetle?🪲</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ien7l3/does_anyone_have_a_polish_recommendation_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1ien0if</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Help picking a go to color</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iry6b29zrdge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1iemyl3</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Gotta love when a polish shines, even in the rain 🌧️</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wwkygmtkrdge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1iemwop</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Best way to do valentine hearts?</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iemwop/best_way_to_do_valentine_hearts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1iems59</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>From Dusk Til Dune Dupe?</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iems59/from_dusk_til_dune_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1iemhwm</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>My first PPU order just arrived!💖</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/spmsi9s2odge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1iemd1b</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Let’s hear your Sassy Sauce tips!</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iemd1b/lets_hear_your_sassy_sauce_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1iem8e4</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Project Polish Updates - 2024, and first month of 2025</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iem8e4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1iem62z</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Drugstore glitter grabber?</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iem62z/drugstore_glitter_grabber/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1iem2v9</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Topcoat experiment with Mooncat Star Wars: A Galaxy Far, Far Away</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3hw31t02ldge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1ielxpd</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Least damaging salon manicure to strengthen nails?</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ielxpd/least_damaging_salon_manicure_to_strengthen_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1ieln3b</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Another Lunar New Year manicure 🎆🧧</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pf2h9teshdge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1iel5xi</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Orly Color Pass 2025 theme Predictions and Speculation</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iel5xi/orly_color_pass_2025_theme_predictions_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1iel3l1</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Clionadh Psilocin &amp; Psilocybin</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x5d7r0nrddge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1iekts3</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Glow in the dark</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iekts3/glow_in_the_dark/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1iekl98</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>My Zoya sale order has arrived ⭐</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iekl98</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1iek643</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Manicurist n00b - finally getting better at my home manis!</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3vul1dgu6dge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1iek4yh</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Coworker asked if my nails were gel. I'm so pleased</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iek4yh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1iejxsz</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Philly Eagles Color Dupe?</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iejxsz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1iejwtf</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Finally trying the famous Psilocybin! 🥰</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iejwtf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1iejvcw</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>RIP to nail colors in uniform. It was fun while it lasted 😔</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iejvcw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1iejd4a</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Just trying new polishes 😁</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iejd4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1iejcev</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>W7 Aurelia</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iejcev</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1iej42y</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Pigment of my Imagination vs Deep Space?</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iej42y/pigment_of_my_imagination_vs_deep_space/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1ieid8w</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>“Cock-a-doodle-doom” Sassy Sauce 🥵</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ieid8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1iehywq</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Linear holographic orange?</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iehywq/linear_holographic_orange/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1iehleo</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Starrily/Mooncat combo</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iehleo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1iehfvu</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Is anyone looking for this holo taco collection?</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nq0ozxjgmcge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1iegox2</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Still working on this look</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iegox2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1iegb9a</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Oh, whooo is shee? 🔍</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iegb9a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1iefkq2</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Hot Syrup, Autumn &amp; Eternity.</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iefkq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1iee3ms</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Sweet Potato SMASHed it!</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iee3ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1ieat43</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Jade nails for Lunar New Year 🧧</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ce8wo6h7page1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1if1n4f</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Do it yourself ❤️🥳</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1if1n4f/do_it_yourself/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1if15wr</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Wanted to share my artwork!</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if15wr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1if0len</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>💋✨</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if0len</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1if0ie2</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Cute nails for Valentine date</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n8rxtx544hge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1iez0ko</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>🧼🍬🧬🫧🛼 decently proud of these 🎀</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iez0ko</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1iexgnj</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>I am proud of these!</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iexgnj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1iewtwp</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>My interpretation of valentines nails</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ftydctm0gge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1iewbjt</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Any ideas for the next ones? Valentines theme?</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vn474sqnvfge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1iew9er</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Red o silver?</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gvgy9ao3vfge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1iew913</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Purple or pink</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c68a3420vfge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1ievvml</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Finished my critter nail set 🐛 🍄 🔮 🐸 it's not the prettiest set but it was so fun to make!</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ievvml</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1ieviom</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Yet another Valentine’s set 💌</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kj489g05ofge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1ieuvn7</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>dior saddle bag!</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ieuvn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1ieupo3</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>lunar new year lion tutorial</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ad80752rgfge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1ieuoq4</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>smiski nails</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ieuoq4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1ieumg5</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>JuSt gOt nEw nAiLs</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hismkt2yffge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1iesjc7</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Japanese Themed Nails</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iesjc7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1ies9gq</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>So I did my first press ons</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ies9gq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1ierofz</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Valentine vibe</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ierofz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1ieqhvk</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Did some gel-x nails and painted some spooky designs</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/he2yb4qeiege1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1ieqboh</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Purple chromeeee</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8o0tbsd3hege1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1iep0dv</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Some recent ones I've done. (Beginner)</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iep0dv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1ieoasu</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Valentine Frenchies @spiritfinger_nails</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bnu6u11p1ege1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1ienu70</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Hearts on my nails for Valentine’s ❤️💅 What do you think?</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s3w24548ydge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1ien7ts</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Pastel bugs and bones</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ien7ts</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1iej5oh</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>My friend thanked me with this gorgeous manicure!</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/io1d82w9zcge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1ien3u7</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Birthday and Valentine's</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xxmvk11psdge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1iemehw</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>How do my gel x nails look</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dst319tgndge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1ielmwb</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Scaled and icy inspired</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ielmwb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1iekmjh</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>collection of my fav sets 💅🏼</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iekmjh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1iekkxs</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Need inspo for nude designs!</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1iekkxs/need_inspo_for_nude_designs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1ieju1g</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Worm nails</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ieju1g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1iejf1l</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Flower and ocean</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51whynsi1dge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1iejdye</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Cherrys</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rkdmr6ua1dge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1ieiuxz</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Simple, delicate and many colors</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dl6vc0fbxcge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1ieih78</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Chrome powder is hard</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ieih78</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1ieh2tt</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qk6p5azkjcge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1iegwj2</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Throw back of Halloween design</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iegwj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1iega3w</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>3 Valentines Sets. Which one is your fav? 💘</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iega3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1ied7pd</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Still in cute winter mode</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ied7pd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1ieapug</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>3D cherries 🍒</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/trbrxk50oage1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Feb  2 08:09:22 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_02.xlsx
+++ b/data/collected_data/2025_02_02.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1308"/>
+  <dimension ref="A1:C1516"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22669,6 +22669,3542 @@
         </is>
       </c>
     </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1ifs0b0</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>How can I make my nails look more feminine?</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifs0b0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1ifrz4h</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>How do these look? This is my dominant hand</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifrz4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1ifrvnf</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>🩷💚</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ifrvnf/_/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1ifrnwl</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>First time getting cat eye!</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifrnwl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1ifr6sd</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>ready for vday 🩷</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gnqiie437oge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1ifqu2r</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Happy lunar new year: year of the wood snake!</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmmo38t23oge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1ifqm57</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Red chrome</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wqww3cco0oge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1ifqgw1</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Trying some talons - they’re fun but I will not be able to pick my nose with this set 😂</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/53xpch61znge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1ifpk3k</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>My valentines set! I can’t believe l couldn’t find any references with acrylic hearts! It was my nail techs first time and she ate🙌🏻</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7q3dci5pnge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1ifp72s</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>February Nails</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ijj1tmclnge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1ifovm4</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Is this worth $135</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifovm4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1ifop7s</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Valentines Day Set💌</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbhm70cdgnge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1ifomm8</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Been doing my own nails for about a year now, this is my most recent set!</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2e03935ofnge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1ifokuy</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>My Valentine’s Day “Sweetheart Candy” Set 🩷</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8rvi8ke6fnge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1ifobeu</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>natural nails advice please</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifobeu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1ifo6md</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Ready for Valentines Day ❤️</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5q07za28bnge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1ifnsw0</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>First Valentines Day set</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifnsw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1ifnl45</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>What is the white thing at the bottom of my ring fingernail? It’s not coming off</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9pbrno55nge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1ifmxr1</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>these nail stickers are the way</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifmxr1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1ifmtj0</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>First time getting nail extensions</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c77bmotsxmge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1ifmryb</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>First time getting nail extensions</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izjji5zcxmge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1ifmj84</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>2nd try for a DIY girl</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifmj84</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1ifmire</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>MY VALENTINE NAILS</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okew0bswumge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1ifmgd3</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>First attempt at powder nail dip</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zehkzr3aumge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1ifm8ea</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Marble ✨</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3yk6vyx6smge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1ifm6b3</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>My best friend is my nail tech</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifm6b3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1ifm2hp</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Tell me what you think 🤔</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4l9uxe4oqmge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1iflvx9</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>What do you think of my nails?</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n2u7y1pxomge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1iflldm</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Love ❤️</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vnfzicl8mmge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1ifli7m</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Valentines meets conclave</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifli7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1iflabd</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Birthday Nails 🎉💅</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iflabd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1ifl99e</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>I sketched my wedding anniversary/Valentines day nails and my nail tech did the dang THANG 🫶🏼♥️😤 I hope y’all have nail techs who like to get creative with you 💖</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifl99e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1ifkzpa</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Does this count as a valentine set??</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqy5gs9sgmge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1ifkwoz</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Black!</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifkwoz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1ifkpht</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>First time with a blue and not square round.</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gg2x01l9emge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1ifkcgf</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Finished product vs the inspiration.</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifkcgf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1ifk0iu</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Red jelly nails 🌶️</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifk0iu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1ifjzj3</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Looking for dupe!</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hx7412j18mge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1ifjq7u</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>This week's color</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vhoextet5mge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1ifju9m</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Valentine's day set 💕</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifju9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1ifjs3f</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>This is the closest I will ever get to Valentine’s Day nails.</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifjs3f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1ifjokc</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>This works wonders for thin nails!</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z2z0lkke5mge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1ifiu7e</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Jello Jello base coat help</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ifiu7e/jello_jello_base_coat_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1ifiw94</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>This is my favorite manicure I’ve ever done 😍</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/29hdce7tylge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1ifiqy0</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Ale will always be the best doing nails</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hhmf9c4kxlge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1ifipz3</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>New set 💙🩶🤍</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dtqk8e2cxlge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1ifipyw</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Valentine’s Nails✨💕</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxlfqx2cxlge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1ifiokx</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>first set of 2025!</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wshjusa0xlge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1ifhphx</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>DIY Valentine’s Nails 😻😻</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifhphx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1ifh7rf</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Gel Manicure for a Nail Biter</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifh7rf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1ifh3bj</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Perfect jelly milky pink 🥛 🌸</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/os8epd14klge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1ifgu5j</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Nothing beats a warm fire and pretty nails</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ppah5bh3ilge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1ifgtgm</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Gel painted press ons</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifgtgm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1ifg9kk</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Elevated French Tip</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5qvtqcridlge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1ifg7o3</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>My nail tech ruined my nails—they’re as thin as paper now.</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/25ntssq4dlge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1ifg4wt</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Press ons!</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n0e4ceiiclge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1iffo23</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Why don’t press ons work for me?</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iffo23/why_dont_press_ons_work_for_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1iffzet</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>(press on) Queen of Hearts nails for Valentine's Day ❤️</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yd7whicablge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1iffz7p</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Red Roses by Gelish ❤️</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/om5snkg7blge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1iffyoa</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>New favorite color</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iffyoa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1iffxr7</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Finished Painting a Castlevania Valentine Set for my sister! 🫶🏼 (Hence them not fitting they are not sized for me 😆🥰)</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i8e7d5nwalge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1iffx40</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>first attempt at the stained glass look 🙂</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iffx40</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1ifffd5</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Where do you buy isopropyl alcohol?</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ifffd5/where_do_you_buy_isopropyl_alcohol/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1iffexi</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Gel Decals</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iffexi/gel_decals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1iff8xk</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Super new to this but here’s some of my first work. Think I overdid the glitter a bit.</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iff8xk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1ifeuvu</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Cateye manicure</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifeuvu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1ifengx</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Playing around with subtle valentines designs- think I found the design, unsure on which color looks nicer for base?</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ano3i2s0lge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1ifei6e</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>A little late but my 2024 holiday nails</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/az5uc34nzkge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1ifebm1</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>Made this freestyle set for a lipgloss formulator 😍</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ijmntwg7ykge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1ife9qz</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Love this simple set (thin gold chrome at base)</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ife9qz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1ifdvn9</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Need help with finding right press ons</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7iyvfaqrukge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1ifdppo</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Nail advice needed</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ifdppo/nail_advice_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1ifd5ct</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Best nail shape theory</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifd5ct</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1ifcvoh</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>what is this?</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifcvoh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1ifca32</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Opinions please: is this nail shape too pointy/narrow for my chubby fingers? I shaped them like this last night but regret it this morning. Wearing Seche Clear only.</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l53i1zufikge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1ifaz51</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>recent nail art ~</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wjo2elgi8kge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1ifbmu2</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Rosy</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ch1y9cbldkge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1ifbm5e</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Valentine’s nails!💕</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4ng12zfdkge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1ifbixx</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>"I got a new job at Ikea" say less</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cw8qpx1sckge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1ifbjg2</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Butterflies 🦋</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifbjg2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1ifbh2l</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Growth tips🙏</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65qxhaadckge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1ifbex3</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Happy February 💗</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5dlcmhrxbkge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1ifb909</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>My own design</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifb909</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1ifb6v6</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>A beauty even without the sun</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wqkj8g17akge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1ifaoi0</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ja6qlyja6kge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1ifahn2</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Nail Appreciation ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifahn2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1ifad99</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>My newest set! What do you think? 🍒🤍🖤</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wbrfks9u3kge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1ifabrb</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>3d lipssss</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yvu5718j3kge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1ifa9r9</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>I’m obsessed!</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifa9r9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1ifa5bf</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Using foil glue for the first time, have some questions...</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8q0u3f32kge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1if9xia</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>I was stressed so I did these</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/48npeq6d0kge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1if9w16</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Used higher quality gel products for the first time for a classic red!</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qqegavi10kge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1if9vjq</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>Feb nails with a bit of sparkle - thoughts?</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3wgujdxzjge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1if9j5w</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>I haven't done my nails in 5 years so I thought I'd try out all my colours!</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2gowmpq5xjge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1if2twa</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>How do I keep my nails from lifting off?</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1if2twa/how_do_i_keep_my_nails_from_lifting_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1if5shf</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Does this nail shape suit me?</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvtorerqzige1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1if6zvq</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Help, acrylic got caught and fell. I have an infill booked for Friday, should I try to get it done sooner?</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5vv704tcbjge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1if8qrq</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>First time at a nail salon</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1if8qrq/first_time_at_a_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1if95nu</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>my nails are ruined</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rz9tsqq3ujge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1if91br</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Subtle Valentine's Nails</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if91br</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1ifrcuo</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Keeping peel off base in place at night?</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ifrcuo/keeping_peel_off_base_in_place_at_night/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1ifk6zv</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Pure silver/metallic nail polish</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ifk6zv/pure_silvermetallic_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1ifqte1</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Happy year of the wood snake!</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xb74tequ2oge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1ifpx7m</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Mooncat Freshly Bitten</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifpx7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1ifpsua</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>i feel like a 2000's gimmick barbie 😍</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rjim1t0prnge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1ifoshd</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>Painted her nails, did I do good?</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qbbsxh68hnge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1ifoqra</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>January wrap up - with dates!</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifoqra</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1ifoke0</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>First time using a shimmer topper - I love it!</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifoke0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1ifoa7t</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>Candy Moyo crackle?</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35ph20f8cnge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1ifnxtd</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>Found my preferred nail polish finish!</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifnxtd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1ifnkbw</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>sassy sauce referral</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ifnkbw/sassy_sauce_referral/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1ifni9u</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>The Boulevard</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifni9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1ifnfz1</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>Pink and green moment</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifnfz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1ifn8z2</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>I used stickers for the first time!</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzxkd38y1nge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1ifn88l</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Let's play a game: which polish is this?</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifn88l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1ifmryi</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>I’m (still) Not Really A Waitress</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ssfbhx5dxmge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1ifmp8m</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>January Mani Round Up!</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifmp8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1ifmgn6</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>Builder gel on Natural nails feat Lurid Lacquer</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifmgn6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1iflnzw</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>More 2024 manis</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iflnzw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1iflkkd</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>Not mad at it, but not the color I thought it would be...</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iflkkd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1ifljho</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>What are your favorite brands of nail polish that are long lasting?</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ifljho/what_are_your_favorite_brands_of_nail_polish_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1iflgw1</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>Matchy matchy 🍇</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qm20vzdkmge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1ifkpvd</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Birthday mani💕 w my fave polish of all time 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifkpvd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1ifkko7</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>Pink strawberry puffs by cracked 🍓✨</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aowa6nv2dmge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1ifk466</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>Twin peaks inspired nails</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h71egoe49mge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1ifjdu6</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>Day 2 of 14 days of Valentine’s inspo 💕 a pastel skittle</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifjdu6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1ifjazp</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>Illusionist really is that girl</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifjazp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1ifiy67</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>I had too much time on my hands in January</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifiy67</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1ifisnv</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>Jello Jello base coat help</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ifisnv/jello_jello_base_coat_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1ifigid</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>January Manis ✨️</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifigid</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1ifieeu</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>Dreaded air bubbles🥲🫧</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifieeu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1ifhuru</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>A stunner from January's PPU</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ka3d8yx7qlge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1ifhsge</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>February Mani</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifhsge</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1ifhrmw</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>Best plum shades available in canada?</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ifhrmw/best_plum_shades_available_in_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1ifhfn3</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>tropical heatwave in February</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifhfn3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1ifh6ws</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>Steep Dreams by Holo Taco</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ifh6ws/steep_dreams_by_holo_taco/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1ifgvx0</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>Merry February</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zvq7q7chilge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1ifgu5m</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>How to</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/riqitck3ilge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1ifgd26</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>The many manis of January</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifgd26</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1ifg52w</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>Football x Lacquer crossover Playoff nail compilation</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifg52w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1iffoic</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>January Recap 🗓️💅</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dxyv87yt8lge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1iffb7g</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>Zoya Payton</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4l6dk4y5lge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1iff1hu</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>My Wife Picks My Mani: Part 6</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iff1hu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1ifegrj</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>✊️🏳️‍⚧️Trans Rights🏳️‍⚧️✊️</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifegrj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1ifdv7w</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>some brightness for february</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifdv7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1ifdtfj</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>January Manis ❄️</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifdtfj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1ifdrsj</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>First of many Valentine's manis for the next couple of weeks</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/myn8khnwtkge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>1ifdrcy</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>Opi original nail strengthener</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ifdrcy/opi_original_nail_strengthener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>1ifdk77</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>please help me pick 1 brown for my first HT order 😭 feel free to reply with pics if you’ve worn any of them before!!</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifdk77</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>1ifdj48</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>Help me find my undertone?</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifdj48</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>1ifdfwc</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>Dupe for Amanita Moment?</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ifdfwc/dupe_for_amanita_moment/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>1ifd7rp</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>Shimmers!</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jh2jb2ckpkge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>1ifd0pp</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Nails (pretty mismatched but I still like them)</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifd0pp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>1ifd0pl</t>
+        </is>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>Polish help needed</t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ifd0pl/polish_help_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>1ifczrm</t>
+        </is>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>Accidentally distracting myself</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifczrm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>1ifcnos</t>
+        </is>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>Super quick bedtime mani 🍒</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifcnos</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>1ifbxpg</t>
+        </is>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>Colors like ILNP Eclipse??</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ifbxpg/colors_like_ilnp_eclipse/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr">
+        <is>
+          <t>1ifbwig</t>
+        </is>
+      </c>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>Where did all the blue go?</t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifbwig</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>1ifbqme</t>
+        </is>
+      </c>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t>Sunset Clouds</t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7jubt21fekge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>1ienzy6</t>
+        </is>
+      </c>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>nails for brunettes</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rsjey74gzdge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="inlineStr">
+        <is>
+          <t>1ieomo7</t>
+        </is>
+      </c>
+      <c r="B1469" t="inlineStr">
+        <is>
+          <t>Formlahyde in nail hardener</t>
+        </is>
+      </c>
+      <c r="C1469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ieomo7/formlahyde_in_nail_hardener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" t="inlineStr">
+        <is>
+          <t>1iexuvm</t>
+        </is>
+      </c>
+      <c r="B1470" t="inlineStr">
+        <is>
+          <t>ILNP Crystal mani ✨</t>
+        </is>
+      </c>
+      <c r="C1470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iexuvm/ilnp_crystal_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" t="inlineStr">
+        <is>
+          <t>1if6mte</t>
+        </is>
+      </c>
+      <c r="B1471" t="inlineStr">
+        <is>
+          <t>IRL difference between Emily de Molly’s Written Invitation vs Fancy Gloss’s Glowing Mushroom?</t>
+        </is>
+      </c>
+      <c r="C1471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1if6mte/irl_difference_between_emily_de_mollys_written/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" t="inlineStr">
+        <is>
+          <t>1if8j4a</t>
+        </is>
+      </c>
+      <c r="B1472" t="inlineStr">
+        <is>
+          <t>January Manicures 💅🏾 🩵</t>
+        </is>
+      </c>
+      <c r="C1472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if8j4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" t="inlineStr">
+        <is>
+          <t>1ifajul</t>
+        </is>
+      </c>
+      <c r="B1473" t="inlineStr">
+        <is>
+          <t>January Roundup 💃</t>
+        </is>
+      </c>
+      <c r="C1473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifajul</t>
+        </is>
+      </c>
+    </row>
+    <row r="1474">
+      <c r="A1474" t="inlineStr">
+        <is>
+          <t>1ifa674</t>
+        </is>
+      </c>
+      <c r="B1474" t="inlineStr">
+        <is>
+          <t>lunar new year mani🍊🧚🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C1474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l6u7whaa2kge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1475">
+      <c r="A1475" t="inlineStr">
+        <is>
+          <t>1if9z1l</t>
+        </is>
+      </c>
+      <c r="B1475" t="inlineStr">
+        <is>
+          <t>Color like this?</t>
+        </is>
+      </c>
+      <c r="C1475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxflmqgp0kge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1476">
+      <c r="A1476" t="inlineStr">
+        <is>
+          <t>1if9u9b</t>
+        </is>
+      </c>
+      <c r="B1476" t="inlineStr">
+        <is>
+          <t>L.A. Colors Super Bloom</t>
+        </is>
+      </c>
+      <c r="C1476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5m6xp47nzjge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1477">
+      <c r="A1477" t="inlineStr">
+        <is>
+          <t>1if9mk4</t>
+        </is>
+      </c>
+      <c r="B1477" t="inlineStr">
+        <is>
+          <t>It really is magical</t>
+        </is>
+      </c>
+      <c r="C1477" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2m3lcmdxxjge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1478">
+      <c r="A1478" t="inlineStr">
+        <is>
+          <t>1if9jff</t>
+        </is>
+      </c>
+      <c r="B1478" t="inlineStr">
+        <is>
+          <t>It’s my Birthstone!</t>
+        </is>
+      </c>
+      <c r="C1478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if9jff</t>
+        </is>
+      </c>
+    </row>
+    <row r="1479">
+      <c r="A1479" t="inlineStr">
+        <is>
+          <t>1if9gmu</t>
+        </is>
+      </c>
+      <c r="B1479" t="inlineStr">
+        <is>
+          <t>january mani round up!</t>
+        </is>
+      </c>
+      <c r="C1479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if9gmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1480">
+      <c r="A1480" t="inlineStr">
+        <is>
+          <t>1if9ejv</t>
+        </is>
+      </c>
+      <c r="B1480" t="inlineStr">
+        <is>
+          <t>You guys influenced me...</t>
+        </is>
+      </c>
+      <c r="C1480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if9e8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1481">
+      <c r="A1481" t="inlineStr">
+        <is>
+          <t>1if8ixe</t>
+        </is>
+      </c>
+      <c r="B1481" t="inlineStr">
+        <is>
+          <t>Well, space isn’t an issue anymore😅</t>
+        </is>
+      </c>
+      <c r="C1481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pws5p7vojge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1482">
+      <c r="A1482" t="inlineStr">
+        <is>
+          <t>1if8afy</t>
+        </is>
+      </c>
+      <c r="B1482" t="inlineStr">
+        <is>
+          <t>The cutest lil guy</t>
+        </is>
+      </c>
+      <c r="C1482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tyglq0cvmjge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1483">
+      <c r="A1483" t="inlineStr">
+        <is>
+          <t>1if88jz</t>
+        </is>
+      </c>
+      <c r="B1483" t="inlineStr">
+        <is>
+          <t>January’s manicures (Jani’s manis)</t>
+        </is>
+      </c>
+      <c r="C1483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if88jz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1484">
+      <c r="A1484" t="inlineStr">
+        <is>
+          <t>1if81m5</t>
+        </is>
+      </c>
+      <c r="B1484" t="inlineStr">
+        <is>
+          <t>Mooncat A Galaxy Far Far Away</t>
+        </is>
+      </c>
+      <c r="C1484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if81m5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1485">
+      <c r="A1485" t="inlineStr">
+        <is>
+          <t>1if7oda</t>
+        </is>
+      </c>
+      <c r="B1485" t="inlineStr">
+        <is>
+          <t>When HR Says No Photos</t>
+        </is>
+      </c>
+      <c r="C1485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if7oda</t>
+        </is>
+      </c>
+    </row>
+    <row r="1486">
+      <c r="A1486" t="inlineStr">
+        <is>
+          <t>1if7er1</t>
+        </is>
+      </c>
+      <c r="B1486" t="inlineStr">
+        <is>
+          <t>dupe for BKL this is caelid?</t>
+        </is>
+      </c>
+      <c r="C1486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1if7er1/dupe_for_bkl_this_is_caelid/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1487">
+      <c r="A1487" t="inlineStr">
+        <is>
+          <t>1if6kk5</t>
+        </is>
+      </c>
+      <c r="B1487" t="inlineStr">
+        <is>
+          <t>“Aurora” from Daisy Chain Polish</t>
+        </is>
+      </c>
+      <c r="C1487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/soclbwwh7jge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1488">
+      <c r="A1488" t="inlineStr">
+        <is>
+          <t>1if5r7h</t>
+        </is>
+      </c>
+      <c r="B1488" t="inlineStr">
+        <is>
+          <t>Give me my agony by Bees Knees Lacquer</t>
+        </is>
+      </c>
+      <c r="C1488" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iyzgqrp9zige1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1489">
+      <c r="A1489" t="inlineStr">
+        <is>
+          <t>1if40rs</t>
+        </is>
+      </c>
+      <c r="B1489" t="inlineStr">
+        <is>
+          <t>PPU Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C1489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1if40rs/ppu_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1490">
+      <c r="A1490" t="inlineStr">
+        <is>
+          <t>1if2vjm</t>
+        </is>
+      </c>
+      <c r="B1490" t="inlineStr">
+        <is>
+          <t>Yes to the shift! ❤️❤️</t>
+        </is>
+      </c>
+      <c r="C1490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if2vjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1491">
+      <c r="A1491" t="inlineStr">
+        <is>
+          <t>1if21ez</t>
+        </is>
+      </c>
+      <c r="B1491" t="inlineStr">
+        <is>
+          <t>Just bought this stand and I love it + new project</t>
+        </is>
+      </c>
+      <c r="C1491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7fnowduxnhge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1492">
+      <c r="A1492" t="inlineStr">
+        <is>
+          <t>1ifpuwi</t>
+        </is>
+      </c>
+      <c r="B1492" t="inlineStr">
+        <is>
+          <t>Encapsulated dried flowers inspired by lockets</t>
+        </is>
+      </c>
+      <c r="C1492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifpuwi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1493">
+      <c r="A1493" t="inlineStr">
+        <is>
+          <t>1ifp8v6</t>
+        </is>
+      </c>
+      <c r="B1493" t="inlineStr">
+        <is>
+          <t>Just a lil guy 🐍</t>
+        </is>
+      </c>
+      <c r="C1493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4n6wcj7ulnge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1494">
+      <c r="A1494" t="inlineStr">
+        <is>
+          <t>1ifovea</t>
+        </is>
+      </c>
+      <c r="B1494" t="inlineStr">
+        <is>
+          <t>Dark Ombré</t>
+        </is>
+      </c>
+      <c r="C1494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifovea</t>
+        </is>
+      </c>
+    </row>
+    <row r="1495">
+      <c r="A1495" t="inlineStr">
+        <is>
+          <t>1ifondn</t>
+        </is>
+      </c>
+      <c r="B1495" t="inlineStr">
+        <is>
+          <t>My Valentine’s Day “Sweethearts Candy” Set 🩷</t>
+        </is>
+      </c>
+      <c r="C1495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxn2cootfnge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1496">
+      <c r="A1496" t="inlineStr">
+        <is>
+          <t>1ifogaw</t>
+        </is>
+      </c>
+      <c r="B1496" t="inlineStr">
+        <is>
+          <t>Nail Art Sticker Rich</t>
+        </is>
+      </c>
+      <c r="C1496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xchkos4wdnge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1497">
+      <c r="A1497" t="inlineStr">
+        <is>
+          <t>1ifnjv5</t>
+        </is>
+      </c>
+      <c r="B1497" t="inlineStr">
+        <is>
+          <t>💜</t>
+        </is>
+      </c>
+      <c r="C1497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e5dqu8ny4nge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1498">
+      <c r="A1498" t="inlineStr">
+        <is>
+          <t>1iflxaz</t>
+        </is>
+      </c>
+      <c r="B1498" t="inlineStr">
+        <is>
+          <t>Some more flowers</t>
+        </is>
+      </c>
+      <c r="C1498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iflxaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1499">
+      <c r="A1499" t="inlineStr">
+        <is>
+          <t>1ifloo4</t>
+        </is>
+      </c>
+      <c r="B1499" t="inlineStr">
+        <is>
+          <t>Strawberry Valentines Nails</t>
+        </is>
+      </c>
+      <c r="C1499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/neooeqh2nmge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1500">
+      <c r="A1500" t="inlineStr">
+        <is>
+          <t>1iflk5m</t>
+        </is>
+      </c>
+      <c r="B1500" t="inlineStr">
+        <is>
+          <t>🩷💚</t>
+        </is>
+      </c>
+      <c r="C1500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rm3y1cnxlmge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1501">
+      <c r="A1501" t="inlineStr">
+        <is>
+          <t>1ifgx2j</t>
+        </is>
+      </c>
+      <c r="B1501" t="inlineStr">
+        <is>
+          <t>Some of my best work</t>
+        </is>
+      </c>
+      <c r="C1501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifgx2j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1502">
+      <c r="A1502" t="inlineStr">
+        <is>
+          <t>1iffxe7</t>
+        </is>
+      </c>
+      <c r="B1502" t="inlineStr">
+        <is>
+          <t>Finished Painting a Castlevania Valentine Set for my sister! 🫶🏼 (Hence them not fitting they are not sized for me 😆🥰)</t>
+        </is>
+      </c>
+      <c r="C1502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n19ugggtalge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1503">
+      <c r="A1503" t="inlineStr">
+        <is>
+          <t>1ifftzz</t>
+        </is>
+      </c>
+      <c r="B1503" t="inlineStr">
+        <is>
+          <t>Using foil glue for the first time, have some questions...</t>
+        </is>
+      </c>
+      <c r="C1503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cwd11az1alge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1504">
+      <c r="A1504" t="inlineStr">
+        <is>
+          <t>1ifew92</t>
+        </is>
+      </c>
+      <c r="B1504" t="inlineStr">
+        <is>
+          <t>Quilting Nails @ a Japanese Nail Salon</t>
+        </is>
+      </c>
+      <c r="C1504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifew92</t>
+        </is>
+      </c>
+    </row>
+    <row r="1505">
+      <c r="A1505" t="inlineStr">
+        <is>
+          <t>1ifegrr</t>
+        </is>
+      </c>
+      <c r="B1505" t="inlineStr">
+        <is>
+          <t>I love this set so much, idk why, they give alt bimbo</t>
+        </is>
+      </c>
+      <c r="C1505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifegrr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1506">
+      <c r="A1506" t="inlineStr">
+        <is>
+          <t>1ifd4jz</t>
+        </is>
+      </c>
+      <c r="B1506" t="inlineStr">
+        <is>
+          <t>Nail art for beginner/ hobbyist</t>
+        </is>
+      </c>
+      <c r="C1506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ifd4jz/nail_art_for_beginner_hobbyist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1507">
+      <c r="A1507" t="inlineStr">
+        <is>
+          <t>1ifbysm</t>
+        </is>
+      </c>
+      <c r="B1507" t="inlineStr">
+        <is>
+          <t>How to prevent sheer polish from looking streaky</t>
+        </is>
+      </c>
+      <c r="C1507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ifbysm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1508">
+      <c r="A1508" t="inlineStr">
+        <is>
+          <t>1ifbich</t>
+        </is>
+      </c>
+      <c r="B1508" t="inlineStr">
+        <is>
+          <t>"I got a new job at Ikea" say less</t>
+        </is>
+      </c>
+      <c r="C1508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqi5a4cnckge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1509">
+      <c r="A1509" t="inlineStr">
+        <is>
+          <t>1ifbaae</t>
+        </is>
+      </c>
+      <c r="B1509" t="inlineStr">
+        <is>
+          <t>Happy Valentine's Month!</t>
+        </is>
+      </c>
+      <c r="C1509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bm4xqzgxakge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1510">
+      <c r="A1510" t="inlineStr">
+        <is>
+          <t>1if8lm2</t>
+        </is>
+      </c>
+      <c r="B1510" t="inlineStr">
+        <is>
+          <t>Love a bit of leopard!</t>
+        </is>
+      </c>
+      <c r="C1510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if8lm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1511">
+      <c r="A1511" t="inlineStr">
+        <is>
+          <t>1if837t</t>
+        </is>
+      </c>
+      <c r="B1511" t="inlineStr">
+        <is>
+          <t>Ain't this cute🥰</t>
+        </is>
+      </c>
+      <c r="C1511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1vkqkxp6ljge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1512">
+      <c r="A1512" t="inlineStr">
+        <is>
+          <t>1if7u8u</t>
+        </is>
+      </c>
+      <c r="B1512" t="inlineStr">
+        <is>
+          <t>Goth-adjacent stars ⭐️🖤</t>
+        </is>
+      </c>
+      <c r="C1512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if7u8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1513">
+      <c r="A1513" t="inlineStr">
+        <is>
+          <t>1if6ksp</t>
+        </is>
+      </c>
+      <c r="B1513" t="inlineStr">
+        <is>
+          <t>Summer ☀️ fun beelive</t>
+        </is>
+      </c>
+      <c r="C1513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if6ksp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1514">
+      <c r="A1514" t="inlineStr">
+        <is>
+          <t>1if5mis</t>
+        </is>
+      </c>
+      <c r="B1514" t="inlineStr">
+        <is>
+          <t>Cat Eye + Hearts ☺️</t>
+        </is>
+      </c>
+      <c r="C1514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2n09vkcyxige1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1515">
+      <c r="A1515" t="inlineStr">
+        <is>
+          <t>1if5dy1</t>
+        </is>
+      </c>
+      <c r="B1515" t="inlineStr">
+        <is>
+          <t>What do you think of these mismatch nail hearts?</t>
+        </is>
+      </c>
+      <c r="C1515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rwi3513avige1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1516">
+      <c r="A1516" t="inlineStr">
+        <is>
+          <t>1if24ha</t>
+        </is>
+      </c>
+      <c r="B1516" t="inlineStr">
+        <is>
+          <t>My nails 2024</t>
+        </is>
+      </c>
+      <c r="C1516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1if24ha</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>